<commit_message>
Modification de fichier excel de bord 1a et 1b "équipe entière"
</commit_message>
<xml_diff>
--- a/gestion_de_projet/Pilotage_de_projet.xlsx
+++ b/gestion_de_projet/Pilotage_de_projet.xlsx
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="211">
   <si>
     <t xml:space="preserve">TamairOS V0.1</t>
   </si>
@@ -249,19 +249,52 @@
     <t xml:space="preserve">Explication</t>
   </si>
   <si>
+    <t xml:space="preserve">Developpement Projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’OS doit posséder une interface graphique pour gérer les différentes commandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test proto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Developement Projet</t>
   </si>
   <si>
-    <t xml:space="preserve">DP001</t>
+    <t xml:space="preserve">DP003</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
+    <t xml:space="preserve">L’OS doit posséder 5 couches cohérentes et dépendantes les unes des autres</t>
   </si>
   <si>
-    <t xml:space="preserve">l’OS doit utiliser un disque dur virtuel, sous forme de fichier</t>
+    <t xml:space="preserve">Suivi </t>
   </si>
   <si>
-    <t xml:space="preserve">Test proto</t>
+    <t xml:space="preserve">DP004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’OS doit posséder un disque dur virtuel fragmenté sous forme de fichier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’OS peut s’installer à l’aide d’un installeur programmé en JAVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’OS doit être programmé en langage C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suivi</t>
   </si>
   <si>
     <t xml:space="preserve">Gestion de projet</t>
@@ -270,10 +303,28 @@
     <t xml:space="preserve">GP001</t>
   </si>
   <si>
-    <t xml:space="preserve">O</t>
+    <t xml:space="preserve">L’équipe doit tenir à jour un excel de bord chaque semaine</t>
   </si>
   <si>
-    <t xml:space="preserve">l’OS doit &lt;verbe infinitif&gt; &lt;compléments&gt;</t>
+    <t xml:space="preserve">Suivi / Bilan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’équipe doit tenir à jour un espace de travail virtuel (cloud GitHub)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’équipe doit posséder une répartition du travail équitable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réunion </t>
   </si>
   <si>
     <t xml:space="preserve">                    OBS
@@ -8762,9 +8813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>667800</xdr:colOff>
+      <xdr:colOff>667440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8774,7 +8825,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="356760" y="95040"/>
-          <a:ext cx="7918920" cy="340560"/>
+          <a:ext cx="7918560" cy="340200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8826,9 +8877,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>820800</xdr:rowOff>
+      <xdr:rowOff>820440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8838,7 +8889,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13178520" y="3549960"/>
-          <a:ext cx="2889360" cy="558720"/>
+          <a:ext cx="2889000" cy="558360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -8896,9 +8947,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>187560</xdr:colOff>
+      <xdr:colOff>187200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>520920</xdr:rowOff>
+      <xdr:rowOff>520560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8908,7 +8959,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13116600" y="4511880"/>
-          <a:ext cx="2889360" cy="554040"/>
+          <a:ext cx="2889000" cy="553680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -8966,9 +9017,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>282600</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>711000</xdr:rowOff>
+      <xdr:rowOff>710640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8978,7 +9029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13211640" y="2525040"/>
-          <a:ext cx="2889360" cy="558720"/>
+          <a:ext cx="2889000" cy="558360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9036,9 +9087,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>208800</xdr:colOff>
+      <xdr:colOff>208440</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9048,7 +9099,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13137840" y="1785960"/>
-          <a:ext cx="2889360" cy="561960"/>
+          <a:ext cx="2889000" cy="561600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9106,9 +9157,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>265680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9118,7 +9169,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13195080" y="1378440"/>
-          <a:ext cx="2889360" cy="292320"/>
+          <a:ext cx="2889000" cy="291960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9176,9 +9227,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>34920</xdr:colOff>
+      <xdr:colOff>34560</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9188,7 +9239,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16427880" y="566640"/>
-          <a:ext cx="3454560" cy="463680"/>
+          <a:ext cx="3454200" cy="463320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9246,9 +9297,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9258,7 +9309,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16425720" y="1126440"/>
-          <a:ext cx="3528360" cy="494640"/>
+          <a:ext cx="3528000" cy="494280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9332,9 +9383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>689760</xdr:colOff>
+      <xdr:colOff>689400</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9344,7 +9395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16449480" y="47520"/>
-          <a:ext cx="3281760" cy="401400"/>
+          <a:ext cx="3281400" cy="401040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9407,9 +9458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>237600</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9418,8 +9469,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17952480" y="2288160"/>
-          <a:ext cx="3305880" cy="2692440"/>
+          <a:off x="17953200" y="2288160"/>
+          <a:ext cx="3305520" cy="2692080"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9550,9 +9601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>190080</xdr:colOff>
+      <xdr:colOff>189720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9561,8 +9612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15912360" y="326160"/>
-          <a:ext cx="3305880" cy="1191960"/>
+          <a:off x="15912720" y="326160"/>
+          <a:ext cx="3305880" cy="1191600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9645,9 +9696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>654120</xdr:colOff>
+      <xdr:colOff>653760</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9656,8 +9707,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4011840" y="6743520"/>
-          <a:ext cx="3334320" cy="801720"/>
+          <a:off x="4011120" y="6743520"/>
+          <a:ext cx="3333960" cy="801360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9715,9 +9766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>235080</xdr:colOff>
+      <xdr:colOff>234720</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9726,8 +9777,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9194400" y="6812640"/>
-          <a:ext cx="3355200" cy="797040"/>
+          <a:off x="9193680" y="6812640"/>
+          <a:ext cx="3354840" cy="796680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9795,9 +9846,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>256680</xdr:colOff>
+      <xdr:colOff>256320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9806,8 +9857,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13697280" y="6588720"/>
-          <a:ext cx="3306240" cy="801720"/>
+          <a:off x="13696200" y="6588720"/>
+          <a:ext cx="3305520" cy="801360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9885,9 +9936,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>242280</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9896,8 +9947,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14488560" y="1959480"/>
-          <a:ext cx="3306240" cy="844920"/>
+          <a:off x="14487480" y="1959480"/>
+          <a:ext cx="3305520" cy="844560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9970,9 +10021,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>46440</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1058760</xdr:rowOff>
+      <xdr:rowOff>1058400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9981,8 +10032,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17164800" y="2876040"/>
-          <a:ext cx="3349800" cy="820800"/>
+          <a:off x="17164080" y="2876040"/>
+          <a:ext cx="3349440" cy="820440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10055,9 +10106,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1379160</xdr:colOff>
+      <xdr:colOff>1378800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10067,7 +10118,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="525240" y="0"/>
-          <a:ext cx="10950840" cy="514080"/>
+          <a:ext cx="10949400" cy="513720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10119,9 +10170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>46440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>320760</xdr:rowOff>
+      <xdr:rowOff>320400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10130,8 +10181,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17110440" y="969120"/>
-          <a:ext cx="2889000" cy="1740240"/>
+          <a:off x="17109000" y="969120"/>
+          <a:ext cx="2889000" cy="1739880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10194,9 +10245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>707760</xdr:colOff>
+      <xdr:colOff>707400</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10206,7 +10257,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="351720" y="71280"/>
-          <a:ext cx="6923160" cy="381960"/>
+          <a:ext cx="6922800" cy="381600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10258,9 +10309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10270,7 +10321,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3450600" y="1848960"/>
-          <a:ext cx="1599120" cy="575280"/>
+          <a:ext cx="1598760" cy="574920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10353,9 +10404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674640</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10365,7 +10416,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1534320" y="3929760"/>
-          <a:ext cx="1678680" cy="511200"/>
+          <a:ext cx="1678320" cy="510840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10448,9 +10499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>276120</xdr:colOff>
+      <xdr:colOff>275760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10460,7 +10511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4286880" y="3929760"/>
-          <a:ext cx="1750320" cy="511200"/>
+          <a:ext cx="1749960" cy="510840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10543,9 +10594,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>142560</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10555,7 +10606,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6578640" y="3929760"/>
-          <a:ext cx="1742760" cy="511200"/>
+          <a:ext cx="1742400" cy="510840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10632,7 +10683,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>646560</xdr:colOff>
+      <xdr:colOff>646920</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -10640,7 +10691,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>101160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10649,8 +10700,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2563920" y="2242080"/>
-          <a:ext cx="1500120" cy="1872360"/>
+          <a:off x="2565000" y="2242800"/>
+          <a:ext cx="1499760" cy="1872000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10683,7 +10734,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -10691,7 +10742,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>211320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10700,8 +10751,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="3958920" y="2720880"/>
-          <a:ext cx="1500120" cy="914760"/>
+          <a:off x="3959640" y="2721600"/>
+          <a:ext cx="1499760" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10734,7 +10785,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -10742,7 +10793,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>77760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10751,8 +10802,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5100840" y="1578960"/>
-          <a:ext cx="1500120" cy="3198600"/>
+          <a:off x="5101560" y="1579680"/>
+          <a:ext cx="1499760" cy="3198240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10791,9 +10842,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>565920</xdr:colOff>
+      <xdr:colOff>565560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10803,7 +10854,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="555120" y="1857600"/>
-          <a:ext cx="1742760" cy="575280"/>
+          <a:ext cx="1742400" cy="574920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10867,9 +10918,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>639720</xdr:colOff>
+      <xdr:colOff>639360</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10879,7 +10930,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6405840" y="2136240"/>
-          <a:ext cx="1606680" cy="360360"/>
+          <a:ext cx="1606320" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10956,7 +11007,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>101880</xdr:colOff>
+      <xdr:colOff>102240</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
@@ -10964,7 +11015,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>646560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10973,8 +11024,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" rot="16200000">
-          <a:off x="5698800" y="981360"/>
-          <a:ext cx="67320" cy="2962080"/>
+          <a:off x="5698440" y="981720"/>
+          <a:ext cx="66960" cy="2961720"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11060,9 +11111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>666000</xdr:colOff>
+      <xdr:colOff>665640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11072,7 +11123,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3970080" y="1056960"/>
-          <a:ext cx="1651320" cy="318600"/>
+          <a:ext cx="1650960" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11124,9 +11175,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>475560</xdr:colOff>
+      <xdr:colOff>475200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11136,7 +11187,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10643760" y="576000"/>
-          <a:ext cx="2845440" cy="1775520"/>
+          <a:ext cx="2845080" cy="1775160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -11199,9 +11250,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>738360</xdr:colOff>
+      <xdr:colOff>738000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11211,7 +11262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="207000" y="48240"/>
-          <a:ext cx="7098480" cy="381960"/>
+          <a:ext cx="7098120" cy="381600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11263,9 +11314,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:colOff>531000</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11275,7 +11326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3887640" y="1483200"/>
-          <a:ext cx="1599120" cy="359280"/>
+          <a:ext cx="1598760" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11339,9 +11390,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>640800</xdr:colOff>
+      <xdr:colOff>640440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11351,7 +11402,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2774160" y="2304000"/>
-          <a:ext cx="1210320" cy="366840"/>
+          <a:ext cx="1209960" cy="366480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11415,9 +11466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>441360</xdr:colOff>
+      <xdr:colOff>441000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11427,7 +11478,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4992120" y="2304000"/>
-          <a:ext cx="1210320" cy="367200"/>
+          <a:ext cx="1209960" cy="366840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11491,9 +11542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11503,7 +11554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6322680" y="2300760"/>
-          <a:ext cx="1250280" cy="351720"/>
+          <a:ext cx="1249920" cy="351360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11561,7 +11612,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>43200</xdr:colOff>
+      <xdr:colOff>43560</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11569,7 +11620,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>537840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11578,8 +11629,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3806280" y="1422000"/>
-          <a:ext cx="460440" cy="1300680"/>
+          <a:off x="3807360" y="1422720"/>
+          <a:ext cx="460080" cy="1300320"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11612,15 +11663,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
+      <xdr:colOff>539640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>628200</xdr:colOff>
+      <xdr:colOff>628560</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11629,8 +11680,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="4905720" y="1625040"/>
-          <a:ext cx="460440" cy="894960"/>
+          <a:off x="4906080" y="1625760"/>
+          <a:ext cx="460080" cy="894600"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11663,7 +11714,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
+      <xdr:colOff>539280</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11671,7 +11722,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>377640</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11680,8 +11731,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5587920" y="942840"/>
-          <a:ext cx="456840" cy="2256120"/>
+          <a:off x="5588640" y="943560"/>
+          <a:ext cx="456480" cy="2255760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11720,9 +11771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:colOff>531000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11732,7 +11783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3876480" y="935280"/>
-          <a:ext cx="1610280" cy="318600"/>
+          <a:ext cx="1609920" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11784,9 +11835,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>671040</xdr:colOff>
+      <xdr:colOff>670680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11796,7 +11847,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3610080" y="2815200"/>
-          <a:ext cx="1210680" cy="351360"/>
+          <a:ext cx="1210320" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11860,9 +11911,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>671040</xdr:colOff>
+      <xdr:colOff>670680</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11872,7 +11923,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3610080" y="3815280"/>
-          <a:ext cx="1210680" cy="367200"/>
+          <a:ext cx="1210320" cy="366840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11936,9 +11987,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>671040</xdr:colOff>
+      <xdr:colOff>670680</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11948,7 +11999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3610080" y="3319200"/>
-          <a:ext cx="1210680" cy="359280"/>
+          <a:ext cx="1210320" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12006,15 +12057,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>43920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12023,8 +12074,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3386880" y="2672640"/>
-          <a:ext cx="222840" cy="322560"/>
+          <a:off x="3387600" y="2673000"/>
+          <a:ext cx="222480" cy="322200"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12055,9 +12106,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>43920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -12072,8 +12123,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3386880" y="2672280"/>
-          <a:ext cx="222840" cy="1330920"/>
+          <a:off x="3387600" y="2673000"/>
+          <a:ext cx="222480" cy="1330560"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12104,9 +12155,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>43920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -12121,8 +12172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3386880" y="2672280"/>
-          <a:ext cx="222840" cy="826920"/>
+          <a:off x="3387600" y="2673000"/>
+          <a:ext cx="222480" cy="826560"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12159,9 +12210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>582840</xdr:colOff>
+      <xdr:colOff>582480</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12171,7 +12222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10751040" y="383400"/>
-          <a:ext cx="2845440" cy="975600"/>
+          <a:ext cx="2845080" cy="975240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -12229,9 +12280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>473760</xdr:colOff>
+      <xdr:colOff>473400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12241,7 +12292,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="995400" y="2316600"/>
-          <a:ext cx="1210320" cy="366840"/>
+          <a:ext cx="1209960" cy="366480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12305,9 +12356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>499320</xdr:colOff>
+      <xdr:colOff>498960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12317,7 +12368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1826640" y="2817360"/>
-          <a:ext cx="1210680" cy="351360"/>
+          <a:ext cx="1210320" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12375,13 +12426,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>653760</xdr:colOff>
+      <xdr:colOff>654480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>95040</xdr:colOff>
+      <xdr:colOff>95400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
@@ -12392,8 +12443,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2684880"/>
-          <a:ext cx="246960" cy="308520"/>
+          <a:off x="1580400" y="2685600"/>
+          <a:ext cx="246600" cy="308160"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12430,9 +12481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>532800</xdr:colOff>
+      <xdr:colOff>532440</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12442,7 +12493,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1860120" y="3317760"/>
-          <a:ext cx="1210680" cy="351360"/>
+          <a:ext cx="1210320" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12506,9 +12557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>542520</xdr:colOff>
+      <xdr:colOff>542160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12518,7 +12569,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1869840" y="3900600"/>
-          <a:ext cx="1210680" cy="351720"/>
+          <a:ext cx="1210320" cy="351360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12582,9 +12633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>599400</xdr:colOff>
+      <xdr:colOff>599040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12594,7 +12645,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1926720" y="4500720"/>
-          <a:ext cx="1210680" cy="351720"/>
+          <a:ext cx="1210320" cy="351360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12658,9 +12709,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>78120</xdr:colOff>
+      <xdr:colOff>77760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12670,7 +12721,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7808400" y="2302200"/>
-          <a:ext cx="1254240" cy="366840"/>
+          <a:ext cx="1253880" cy="366480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12734,9 +12785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>115920</xdr:colOff>
+      <xdr:colOff>115560</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12746,7 +12797,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8651880" y="2886480"/>
-          <a:ext cx="1254240" cy="351360"/>
+          <a:ext cx="1253880" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12810,9 +12861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>125640</xdr:colOff>
+      <xdr:colOff>125280</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12822,7 +12873,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8661600" y="3410280"/>
-          <a:ext cx="1254240" cy="351360"/>
+          <a:ext cx="1253880" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12880,13 +12931,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>259200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>473760</xdr:colOff>
+      <xdr:colOff>474120</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
@@ -12897,8 +12948,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8436960" y="2670480"/>
-          <a:ext cx="215280" cy="392040"/>
+          <a:off x="8437320" y="2671200"/>
+          <a:ext cx="214920" cy="391680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12929,15 +12980,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>259560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>483480</xdr:colOff>
+      <xdr:colOff>483840</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12946,57 +12997,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8437320" y="2671200"/>
-          <a:ext cx="224640" cy="915840"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:tailEnd len="med" type="arrow" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>653760</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128520</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Connecteur en angle 32"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="1579680" y="2684880"/>
-          <a:ext cx="280440" cy="808920"/>
+          <a:off x="8437680" y="2671560"/>
+          <a:ext cx="224280" cy="915480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13029,23 +13031,23 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>654120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>138240</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:colOff>128520</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="Connecteur en angle 33"/>
+        <xdr:cNvPr id="52" name="Connecteur en angle 32"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2684880"/>
-          <a:ext cx="289800" cy="1392480"/>
+          <a:off x="1580400" y="2685600"/>
+          <a:ext cx="280080" cy="808560"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13076,25 +13078,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>653760</xdr:colOff>
+      <xdr:colOff>654480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>195120</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:colOff>138240</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="Connecteur en angle 34"/>
+        <xdr:cNvPr id="53" name="Connecteur en angle 33"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2685240"/>
-          <a:ext cx="347040" cy="1992240"/>
+          <a:off x="1580760" y="2685240"/>
+          <a:ext cx="289440" cy="1392120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13125,7 +13127,56 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>653760</xdr:colOff>
+      <xdr:colOff>654480</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>195480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Connecteur en angle 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1580400" y="2685600"/>
+          <a:ext cx="346680" cy="1991880"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>654120</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -13133,7 +13184,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>538200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13142,8 +13193,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2896920" y="524520"/>
-          <a:ext cx="472680" cy="3107880"/>
+          <a:off x="2898000" y="525240"/>
+          <a:ext cx="472320" cy="3107520"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13176,15 +13227,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
+      <xdr:colOff>539640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13193,8 +13244,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="6333120" y="197640"/>
-          <a:ext cx="458280" cy="3747600"/>
+          <a:off x="6333480" y="198360"/>
+          <a:ext cx="457920" cy="3747240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13238,9 +13289,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>761400</xdr:colOff>
+      <xdr:colOff>761040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13250,7 +13301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="245160" y="78840"/>
-          <a:ext cx="7083360" cy="381960"/>
+          <a:ext cx="7083000" cy="381600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13302,9 +13353,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>675000</xdr:colOff>
+      <xdr:colOff>674640</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13314,7 +13365,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4023720" y="1435680"/>
-          <a:ext cx="1606680" cy="351720"/>
+          <a:ext cx="1606320" cy="351360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13378,9 +13429,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>602640</xdr:colOff>
+      <xdr:colOff>602280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13390,7 +13441,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1929960" y="2264040"/>
-          <a:ext cx="1210680" cy="351360"/>
+          <a:ext cx="1210320" cy="351000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13454,9 +13505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
+      <xdr:colOff>397080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13466,7 +13517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4121280" y="2264040"/>
-          <a:ext cx="1231560" cy="574560"/>
+          <a:ext cx="1231200" cy="574200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13549,9 +13600,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>510840</xdr:colOff>
+      <xdr:colOff>510480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13561,7 +13612,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5856480" y="2253240"/>
-          <a:ext cx="1221480" cy="359280"/>
+          <a:ext cx="1221120" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13619,7 +13670,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -13627,7 +13678,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13636,8 +13687,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3449520" y="880560"/>
-          <a:ext cx="475560" cy="2288160"/>
+          <a:off x="3449160" y="881280"/>
+          <a:ext cx="475200" cy="2287800"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13670,7 +13721,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>584640</xdr:colOff>
+      <xdr:colOff>585000</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -13678,7 +13729,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>682200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13687,8 +13738,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="4544640" y="1976040"/>
-          <a:ext cx="475560" cy="97560"/>
+          <a:off x="4545720" y="1976760"/>
+          <a:ext cx="475200" cy="97200"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13721,7 +13772,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>682560</xdr:colOff>
+      <xdr:colOff>682920</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -13729,7 +13780,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>688680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13738,8 +13789,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5408280" y="1210680"/>
-          <a:ext cx="464760" cy="1617480"/>
+          <a:off x="5409000" y="1211400"/>
+          <a:ext cx="464400" cy="1617120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13778,9 +13829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>753840</xdr:colOff>
+      <xdr:colOff>753480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13790,7 +13841,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4020120" y="894960"/>
-          <a:ext cx="1689120" cy="318600"/>
+          <a:ext cx="1688760" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13842,9 +13893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>624960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13854,7 +13905,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2766240" y="2767680"/>
-          <a:ext cx="1202760" cy="358920"/>
+          <a:ext cx="1202400" cy="358560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13918,9 +13969,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>624960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13930,7 +13981,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2766240" y="3775320"/>
-          <a:ext cx="1202760" cy="359640"/>
+          <a:ext cx="1202400" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13994,9 +14045,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>624960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14006,7 +14057,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2766240" y="3271320"/>
-          <a:ext cx="1202760" cy="359280"/>
+          <a:ext cx="1202400" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14064,15 +14115,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14081,8 +14132,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2543040" y="2617200"/>
-          <a:ext cx="222840" cy="330480"/>
+          <a:off x="2543760" y="2617560"/>
+          <a:ext cx="222480" cy="330120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14113,15 +14164,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14130,8 +14181,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2543040" y="2617200"/>
-          <a:ext cx="222840" cy="1338480"/>
+          <a:off x="2543760" y="2617560"/>
+          <a:ext cx="222480" cy="1338120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14162,15 +14213,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14179,8 +14230,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2543040" y="2617560"/>
-          <a:ext cx="222840" cy="834480"/>
+          <a:off x="2543760" y="2617920"/>
+          <a:ext cx="222480" cy="834120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14217,9 +14268,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>419760</xdr:colOff>
+      <xdr:colOff>419400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14229,7 +14280,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4978080" y="2983320"/>
-          <a:ext cx="1202760" cy="352080"/>
+          <a:ext cx="1202400" cy="351720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14293,9 +14344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>419760</xdr:colOff>
+      <xdr:colOff>419400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14305,7 +14356,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4978080" y="3487680"/>
-          <a:ext cx="1202760" cy="359280"/>
+          <a:ext cx="1202400" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14369,9 +14420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>479880</xdr:colOff>
+      <xdr:colOff>479520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14381,7 +14432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6631560" y="3938400"/>
-          <a:ext cx="1221120" cy="359640"/>
+          <a:ext cx="1220760" cy="359280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14464,9 +14515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>479880</xdr:colOff>
+      <xdr:colOff>479520</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14476,7 +14527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6631560" y="2911320"/>
-          <a:ext cx="1221120" cy="359280"/>
+          <a:ext cx="1220760" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14540,9 +14591,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>479880</xdr:colOff>
+      <xdr:colOff>479520</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14552,7 +14603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6631560" y="3375720"/>
-          <a:ext cx="1221120" cy="366840"/>
+          <a:ext cx="1220760" cy="366480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14629,15 +14680,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>585000</xdr:colOff>
+      <xdr:colOff>585360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>23040</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14646,8 +14697,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4734360" y="2840400"/>
-          <a:ext cx="243720" cy="827280"/>
+          <a:off x="4735080" y="2840760"/>
+          <a:ext cx="243360" cy="826920"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14678,15 +14729,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14695,8 +14746,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6450480" y="2614320"/>
-          <a:ext cx="181440" cy="477360"/>
+          <a:off x="6450840" y="2614680"/>
+          <a:ext cx="181080" cy="477000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14727,15 +14778,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>585000</xdr:colOff>
+      <xdr:colOff>585360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>23040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14744,8 +14795,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4734360" y="2840400"/>
-          <a:ext cx="243720" cy="323280"/>
+          <a:off x="4735080" y="2840760"/>
+          <a:ext cx="243360" cy="322920"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14776,13 +14827,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
@@ -14793,8 +14844,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6450480" y="2613960"/>
-          <a:ext cx="181440" cy="949320"/>
+          <a:off x="6450840" y="2614680"/>
+          <a:ext cx="181080" cy="948960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14825,15 +14876,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14842,8 +14893,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6450480" y="2614320"/>
-          <a:ext cx="181440" cy="1504800"/>
+          <a:off x="6450840" y="2614680"/>
+          <a:ext cx="181080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14880,9 +14931,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>56160</xdr:colOff>
+      <xdr:colOff>55800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14892,7 +14943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="564480" y="2269080"/>
-          <a:ext cx="1223640" cy="366840"/>
+          <a:ext cx="1223280" cy="366480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14950,7 +15001,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>251280</xdr:colOff>
+      <xdr:colOff>251640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -14958,7 +15009,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14967,8 +15018,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2764080" y="200160"/>
-          <a:ext cx="480600" cy="3654000"/>
+          <a:off x="2763720" y="200880"/>
+          <a:ext cx="480240" cy="3653640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15007,9 +15058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>570960</xdr:colOff>
+      <xdr:colOff>570600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>332640</xdr:rowOff>
+      <xdr:rowOff>332280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15019,7 +15070,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11084400" y="3345480"/>
-          <a:ext cx="3305880" cy="1816200"/>
+          <a:ext cx="3305520" cy="1815840"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -15098,9 +15149,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>662400</xdr:colOff>
+      <xdr:colOff>662040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15110,7 +15161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="557640" y="56160"/>
-          <a:ext cx="8427600" cy="381960"/>
+          <a:ext cx="8426520" cy="381600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15162,9 +15213,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1128600</xdr:colOff>
+      <xdr:colOff>1128240</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15178,7 +15229,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="120600" y="5152680"/>
-          <a:ext cx="10530360" cy="4138920"/>
+          <a:ext cx="10529280" cy="4138560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15199,9 +15250,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>297000</xdr:colOff>
+      <xdr:colOff>296640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15210,8 +15261,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12929040" y="3964680"/>
-          <a:ext cx="3327840" cy="2080080"/>
+          <a:off x="12928320" y="3964680"/>
+          <a:ext cx="3327120" cy="2079720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -15316,9 +15367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3884400</xdr:colOff>
+      <xdr:colOff>3884040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15328,7 +15379,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1899720" y="130680"/>
-          <a:ext cx="8243640" cy="385560"/>
+          <a:ext cx="8243280" cy="385200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15380,9 +15431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>82800</xdr:colOff>
+      <xdr:colOff>82440</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15392,7 +15443,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14341320" y="1107000"/>
-          <a:ext cx="3305880" cy="2047320"/>
+          <a:ext cx="3305520" cy="2046960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -15471,9 +15522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>499680</xdr:colOff>
+      <xdr:colOff>499320</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15483,7 +15534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16138080" y="1330920"/>
-          <a:ext cx="3305880" cy="2046960"/>
+          <a:ext cx="3305520" cy="2046600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -15557,7 +15608,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15602,7 +15653,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15647,7 +15698,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15692,7 +15743,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15737,7 +15788,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15782,7 +15833,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15827,7 +15878,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15872,7 +15923,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15917,7 +15968,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -15962,7 +16013,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -16007,7 +16058,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -16052,7 +16103,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13255560" y="1218960"/>
+          <a:off x="13255920" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -16086,9 +16137,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16097,8 +16148,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15557400" y="278640"/>
-          <a:ext cx="3349800" cy="2051640"/>
+          <a:off x="15558120" y="278640"/>
+          <a:ext cx="3349440" cy="2051280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16523,29 +16574,29 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="173" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B5" s="174" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C5" s="174"/>
       <c r="D5" s="174"/>
       <c r="E5" s="174"/>
       <c r="F5" s="174"/>
       <c r="G5" s="175" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="H5" s="175" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="I5" s="175" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="J5" s="173" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K5" s="173" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16562,7 +16613,7 @@
       <c r="I6" s="177"/>
       <c r="J6" s="178"/>
       <c r="K6" s="179" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16754,39 +16805,39 @@
     </row>
     <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="185" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B5" s="185" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="C5" s="185" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="D5" s="185" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="E5" s="185" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="F5" s="185" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="G5" s="185" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="H5" s="185" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="I5" s="185" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="J5" s="185" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="186" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="B6" s="187"/>
       <c r="C6" s="187"/>
@@ -16800,7 +16851,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="189" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B7" s="190"/>
       <c r="C7" s="190"/>
@@ -16814,12 +16865,12 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A8" s="192" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B8" s="192"/>
       <c r="C8" s="192"/>
       <c r="D8" s="192" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="E8" s="192"/>
       <c r="F8" s="192"/>
@@ -16827,12 +16878,12 @@
       <c r="H8" s="192"/>
       <c r="I8" s="192"/>
       <c r="J8" s="192" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A9" s="189" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="B9" s="190"/>
       <c r="C9" s="190"/>
@@ -16846,12 +16897,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A10" s="192" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B10" s="192"/>
       <c r="C10" s="192"/>
       <c r="D10" s="192" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="E10" s="192"/>
       <c r="F10" s="192"/>
@@ -16859,7 +16910,7 @@
       <c r="H10" s="192"/>
       <c r="I10" s="192"/>
       <c r="J10" s="192" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
@@ -16873,7 +16924,7 @@
       <c r="H11" s="192"/>
       <c r="I11" s="192"/>
       <c r="J11" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
@@ -16887,7 +16938,7 @@
       <c r="H12" s="192"/>
       <c r="I12" s="192"/>
       <c r="J12" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
@@ -16901,12 +16952,12 @@
       <c r="H13" s="192"/>
       <c r="I13" s="192"/>
       <c r="J13" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A14" s="186" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="B14" s="190"/>
       <c r="C14" s="190"/>
@@ -16920,7 +16971,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="189" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="B15" s="190"/>
       <c r="C15" s="190"/>
@@ -16934,12 +16985,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A16" s="192" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="B16" s="192"/>
       <c r="C16" s="192"/>
       <c r="D16" s="192" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E16" s="192"/>
       <c r="F16" s="192"/>
@@ -16949,17 +17000,17 @@
       </c>
       <c r="I16" s="192"/>
       <c r="J16" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A17" s="192" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B17" s="192"/>
       <c r="C17" s="192"/>
       <c r="D17" s="192" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E17" s="192"/>
       <c r="F17" s="192"/>
@@ -16969,37 +17020,37 @@
       </c>
       <c r="I17" s="192"/>
       <c r="J17" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A18" s="192" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="B18" s="192"/>
       <c r="C18" s="192"/>
       <c r="D18" s="192" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E18" s="192"/>
       <c r="F18" s="192"/>
       <c r="G18" s="192"/>
       <c r="H18" s="192" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="I18" s="192"/>
       <c r="J18" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A19" s="192" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B19" s="192"/>
       <c r="C19" s="192"/>
       <c r="D19" s="192" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E19" s="192"/>
       <c r="F19" s="192"/>
@@ -17009,12 +17060,12 @@
       </c>
       <c r="I19" s="192"/>
       <c r="J19" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A20" s="189" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="B20" s="190"/>
       <c r="C20" s="190"/>
@@ -17028,12 +17079,12 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A21" s="192" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B21" s="192"/>
       <c r="C21" s="192"/>
       <c r="D21" s="192" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E21" s="192"/>
       <c r="F21" s="192"/>
@@ -17043,17 +17094,17 @@
       </c>
       <c r="I21" s="192"/>
       <c r="J21" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A22" s="192" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="B22" s="192"/>
       <c r="C22" s="192"/>
       <c r="D22" s="192" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E22" s="192"/>
       <c r="F22" s="192"/>
@@ -17063,17 +17114,17 @@
       </c>
       <c r="I22" s="192"/>
       <c r="J22" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A23" s="192" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="B23" s="192"/>
       <c r="C23" s="192"/>
       <c r="D23" s="192" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E23" s="192"/>
       <c r="F23" s="192"/>
@@ -17083,17 +17134,17 @@
       </c>
       <c r="I23" s="192"/>
       <c r="J23" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A24" s="192" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="B24" s="192"/>
       <c r="C24" s="192"/>
       <c r="D24" s="192" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E24" s="192"/>
       <c r="F24" s="192"/>
@@ -17103,17 +17154,17 @@
       </c>
       <c r="I24" s="192"/>
       <c r="J24" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A25" s="192" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="B25" s="192"/>
       <c r="C25" s="192"/>
       <c r="D25" s="192" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E25" s="192"/>
       <c r="F25" s="192"/>
@@ -17123,17 +17174,17 @@
       </c>
       <c r="I25" s="192"/>
       <c r="J25" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A26" s="192" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B26" s="192"/>
       <c r="C26" s="192"/>
       <c r="D26" s="192" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E26" s="192"/>
       <c r="F26" s="192"/>
@@ -17143,17 +17194,17 @@
       </c>
       <c r="I26" s="192"/>
       <c r="J26" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A27" s="192" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B27" s="192"/>
       <c r="C27" s="192"/>
       <c r="D27" s="192" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E27" s="192"/>
       <c r="F27" s="192"/>
@@ -17163,17 +17214,17 @@
       </c>
       <c r="I27" s="192"/>
       <c r="J27" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A28" s="192" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B28" s="192"/>
       <c r="C28" s="192"/>
       <c r="D28" s="192" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E28" s="192"/>
       <c r="F28" s="192"/>
@@ -17183,17 +17234,17 @@
       </c>
       <c r="I28" s="192"/>
       <c r="J28" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A29" s="192" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="B29" s="192"/>
       <c r="C29" s="192"/>
       <c r="D29" s="192" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E29" s="192"/>
       <c r="F29" s="192"/>
@@ -17203,17 +17254,17 @@
       </c>
       <c r="I29" s="192"/>
       <c r="J29" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A30" s="192" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="B30" s="192"/>
       <c r="C30" s="192"/>
       <c r="D30" s="192" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E30" s="192"/>
       <c r="F30" s="192"/>
@@ -17223,12 +17274,12 @@
       </c>
       <c r="I30" s="192"/>
       <c r="J30" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A31" s="189" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B31" s="190"/>
       <c r="C31" s="190"/>
@@ -17242,12 +17293,12 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A32" s="192" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B32" s="192"/>
       <c r="C32" s="192"/>
       <c r="D32" s="192" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E32" s="192"/>
       <c r="F32" s="192"/>
@@ -17257,7 +17308,7 @@
       </c>
       <c r="I32" s="192"/>
       <c r="J32" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false"/>
@@ -17345,24 +17396,24 @@
     </row>
     <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="185" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="B5" s="194" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C5" s="185" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="D5" s="185" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="E5" s="185" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="186" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B6" s="190"/>
       <c r="C6" s="190"/>
@@ -17371,7 +17422,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="192" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B7" s="192"/>
       <c r="C7" s="192" t="n">
@@ -17379,12 +17430,12 @@
       </c>
       <c r="D7" s="192"/>
       <c r="E7" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A8" s="192" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="B8" s="192"/>
       <c r="C8" s="192" t="n">
@@ -17392,12 +17443,12 @@
       </c>
       <c r="D8" s="192"/>
       <c r="E8" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A9" s="192" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B9" s="192"/>
       <c r="C9" s="192" t="n">
@@ -17405,7 +17456,7 @@
       </c>
       <c r="D9" s="192"/>
       <c r="E9" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
@@ -17417,7 +17468,7 @@
     </row>
     <row r="10" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A10" s="192" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="B10" s="192"/>
       <c r="C10" s="192" t="n">
@@ -17425,12 +17476,12 @@
       </c>
       <c r="D10" s="192"/>
       <c r="E10" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A11" s="192" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B11" s="192"/>
       <c r="C11" s="192" t="n">
@@ -17438,12 +17489,12 @@
       </c>
       <c r="D11" s="192"/>
       <c r="E11" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A12" s="192" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="B12" s="192"/>
       <c r="C12" s="192" t="n">
@@ -17451,7 +17502,7 @@
       </c>
       <c r="D12" s="192"/>
       <c r="E12" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
@@ -17463,7 +17514,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A13" s="192" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B13" s="192"/>
       <c r="C13" s="192" t="n">
@@ -17471,7 +17522,7 @@
       </c>
       <c r="D13" s="192"/>
       <c r="E13" s="192" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
@@ -17623,58 +17674,58 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="72" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E7" s="72"/>
       <c r="F7" s="72"/>
       <c r="G7" s="72"/>
       <c r="H7" s="72"/>
       <c r="I7" s="196" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="J7" s="196"/>
       <c r="K7" s="196"/>
       <c r="L7" s="196"/>
       <c r="M7" s="197" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="73" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D8" s="198" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E8" s="76" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F8" s="76" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G8" s="76" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="H8" s="77" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="I8" s="199" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="J8" s="76" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="K8" s="76" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="L8" s="77" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="M8" s="200" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17693,10 +17744,10 @@
         <v>42864</v>
       </c>
       <c r="F9" s="82" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="G9" s="82" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H9" s="83" t="n">
         <f aca="false">+SUM(H10:H26)</f>
@@ -17725,7 +17776,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D10" s="205" t="n">
         <v>42828</v>
@@ -17735,7 +17786,7 @@
       </c>
       <c r="F10" s="88"/>
       <c r="G10" s="89" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="H10" s="90" t="n">
         <v>14</v>
@@ -17762,7 +17813,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="85" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D11" s="205" t="n">
         <v>42830</v>
@@ -17774,7 +17825,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="89" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="H11" s="90" t="n">
         <v>21</v>
@@ -17801,7 +17852,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D12" s="205" t="n">
         <v>42835</v>
@@ -17813,7 +17864,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="89" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="H12" s="90" t="n">
         <v>10.5</v>
@@ -17838,7 +17889,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D13" s="205" t="n">
         <v>42857</v>
@@ -17847,10 +17898,10 @@
         <v>42858</v>
       </c>
       <c r="F13" s="89" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="G13" s="89" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="H13" s="90" t="n">
         <v>14</v>
@@ -17873,7 +17924,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D14" s="205" t="n">
         <v>42835</v>
@@ -17885,7 +17936,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="89" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H14" s="90" t="n">
         <v>29.4</v>
@@ -17910,7 +17961,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D15" s="205" t="n">
         <v>42839</v>
@@ -17922,7 +17973,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H15" s="90" t="n">
         <v>21</v>
@@ -17945,7 +17996,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D16" s="205" t="n">
         <v>42844</v>
@@ -17957,7 +18008,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H16" s="90" t="n">
         <v>28</v>
@@ -17980,7 +18031,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="85" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D17" s="205" t="n">
         <v>42844</v>
@@ -17992,7 +18043,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H17" s="90" t="n">
         <v>14</v>
@@ -18015,7 +18066,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="85" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D18" s="205" t="n">
         <v>42846</v>
@@ -18027,7 +18078,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H18" s="90" t="n">
         <v>7</v>
@@ -18050,7 +18101,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="85" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D19" s="205" t="n">
         <v>42850</v>
@@ -18059,10 +18110,10 @@
         <v>42851</v>
       </c>
       <c r="F19" s="89" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G19" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H19" s="90" t="n">
         <v>14</v>
@@ -18085,7 +18136,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D20" s="205" t="n">
         <v>42839</v>
@@ -18097,7 +18148,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H20" s="90" t="n">
         <v>21</v>
@@ -18120,7 +18171,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="85" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D21" s="205" t="n">
         <v>42850</v>
@@ -18132,7 +18183,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H21" s="90" t="n">
         <v>14</v>
@@ -18155,7 +18206,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D22" s="205" t="n">
         <v>42852</v>
@@ -18164,10 +18215,10 @@
         <v>42856</v>
       </c>
       <c r="F22" s="89" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="G22" s="89" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H22" s="90" t="n">
         <v>21</v>
@@ -18190,7 +18241,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D23" s="205" t="n">
         <v>42832</v>
@@ -18223,7 +18274,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D24" s="205" t="n">
         <v>42839</v>
@@ -18257,7 +18308,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D25" s="205" t="n">
         <v>42864</v>
@@ -18290,7 +18341,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="93" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="D26" s="208" t="n">
         <v>42864</v>
@@ -18413,7 +18464,7 @@
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="42" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18438,7 +18489,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18463,7 +18514,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="42" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18521,7 +18572,7 @@
       <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.87"/>
@@ -18529,18 +18580,18 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -18559,10 +18610,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
@@ -18677,7 +18728,7 @@
       </c>
       <c r="H9" s="49"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A10" s="50" t="s">
         <v>22</v>
       </c>
@@ -18697,7 +18748,7 @@
       <c r="G10" s="52"/>
       <c r="H10" s="53"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="11" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A11" s="50" t="s">
         <v>27</v>
       </c>
@@ -18706,53 +18757,92 @@
       </c>
       <c r="C11" s="50"/>
       <c r="D11" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="F11" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="51"/>
       <c r="G11" s="52"/>
       <c r="H11" s="53"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>31</v>
+      </c>
       <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
+      <c r="D12" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>26</v>
+      </c>
       <c r="G12" s="52"/>
       <c r="H12" s="53"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
     </row>
     <row r="13" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>33</v>
+      </c>
       <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
+      <c r="D13" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>26</v>
+      </c>
       <c r="G13" s="52"/>
       <c r="H13" s="53"/>
     </row>
     <row r="14" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>35</v>
+      </c>
       <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="51" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="52"/>
       <c r="H14" s="53"/>
-    </row>
-    <row r="15" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
       <c r="A15" s="50"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -18761,25 +18851,76 @@
       <c r="F15" s="51"/>
       <c r="G15" s="52"/>
       <c r="H15" s="53"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>39</v>
+      </c>
       <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
+      <c r="D16" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="51" t="s">
+        <v>41</v>
+      </c>
       <c r="G16" s="52"/>
       <c r="H16" s="53"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
+      <c r="A17" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="18" s="31" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
+      <c r="A18" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="2" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="G1:H1"/>
@@ -20144,21 +20285,21 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="67" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="67"/>
       <c r="F28" s="67" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G28" s="67" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H28" s="67" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I28" s="67" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="K28" s="65"/>
       <c r="L28" s="65"/>
@@ -20166,15 +20307,15 @@
     </row>
     <row r="29" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="68" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D29" s="69"/>
       <c r="E29" s="70"/>
       <c r="F29" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G29" s="71" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="H29" s="71"/>
       <c r="I29" s="71"/>
@@ -20185,12 +20326,12 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C30" s="68" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D30" s="69"/>
       <c r="E30" s="70"/>
       <c r="F30" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G30" s="71"/>
       <c r="H30" s="71"/>
@@ -20202,15 +20343,15 @@
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C31" s="68" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D31" s="69"/>
       <c r="E31" s="70"/>
       <c r="F31" s="71" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="G31" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="H31" s="71"/>
       <c r="I31" s="71"/>
@@ -20221,19 +20362,19 @@
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C32" s="68" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D32" s="69"/>
       <c r="E32" s="70"/>
       <c r="F32" s="71"/>
       <c r="G32" s="71" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H32" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="I32" s="71" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="J32" s="64"/>
       <c r="K32" s="65"/>
@@ -20242,17 +20383,17 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C33" s="68" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D33" s="69"/>
       <c r="E33" s="70"/>
       <c r="F33" s="71"/>
       <c r="G33" s="71" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H33" s="71"/>
       <c r="I33" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J33" s="64"/>
       <c r="K33" s="65"/>
@@ -20261,17 +20402,17 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C34" s="68" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D34" s="69"/>
       <c r="E34" s="70"/>
       <c r="F34" s="71"/>
       <c r="G34" s="71" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H34" s="71"/>
       <c r="I34" s="71" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20291,62 +20432,62 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="30" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="30" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="30" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="67" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="D42" s="67"/>
       <c r="E42" s="67"/>
       <c r="F42" s="67" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G42" s="67" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="H42" s="67" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="I42" s="67" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="J42" s="67" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="K42" s="67" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="L42" s="67" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="M42" s="67" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="N42" s="67" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="O42" s="67" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="P42" s="67" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="68" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D43" s="69"/>
       <c r="E43" s="70"/>
@@ -20356,7 +20497,7 @@
       <c r="I43" s="71"/>
       <c r="J43" s="71"/>
       <c r="K43" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="L43" s="71"/>
       <c r="M43" s="71"/>
@@ -20366,7 +20507,7 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="68" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D44" s="69"/>
       <c r="E44" s="70"/>
@@ -20377,20 +20518,20 @@
       <c r="J44" s="71"/>
       <c r="K44" s="71"/>
       <c r="L44" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="M44" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="N44" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="O44" s="71"/>
       <c r="P44" s="71"/>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="68" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D45" s="69"/>
       <c r="E45" s="70"/>
@@ -20404,26 +20545,26 @@
       <c r="M45" s="71"/>
       <c r="N45" s="71"/>
       <c r="O45" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="P45" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="68" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D46" s="69"/>
       <c r="E46" s="70"/>
       <c r="F46" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G46" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="H46" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="I46" s="71"/>
       <c r="J46" s="71"/>
@@ -20433,12 +20574,12 @@
       <c r="N46" s="71"/>
       <c r="O46" s="71"/>
       <c r="P46" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="68" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D47" s="69"/>
       <c r="E47" s="70"/>
@@ -20446,7 +20587,7 @@
       <c r="G47" s="71"/>
       <c r="H47" s="71"/>
       <c r="I47" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="J47" s="71"/>
       <c r="K47" s="71"/>
@@ -20455,12 +20596,12 @@
       <c r="N47" s="71"/>
       <c r="O47" s="71"/>
       <c r="P47" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="68" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D48" s="69"/>
       <c r="E48" s="70"/>
@@ -20469,7 +20610,7 @@
       <c r="H48" s="71"/>
       <c r="I48" s="71"/>
       <c r="J48" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="K48" s="71"/>
       <c r="L48" s="71"/>
@@ -20477,7 +20618,7 @@
       <c r="N48" s="71"/>
       <c r="O48" s="71"/>
       <c r="P48" s="71" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -20612,7 +20753,7 @@
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="72" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
@@ -20627,25 +20768,25 @@
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="73" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G7" s="76" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="H7" s="77" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20664,10 +20805,10 @@
         <v>42864</v>
       </c>
       <c r="F8" s="82" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="G8" s="82" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H8" s="83" t="n">
         <f aca="false">+SUM(H9:H25)</f>
@@ -20679,7 +20820,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="85" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D9" s="86" t="n">
         <v>42828</v>
@@ -20689,7 +20830,7 @@
       </c>
       <c r="F9" s="88"/>
       <c r="G9" s="89" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="H9" s="90" t="n">
         <v>14</v>
@@ -20700,7 +20841,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D10" s="86" t="n">
         <v>42830</v>
@@ -20712,7 +20853,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="89" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="H10" s="90" t="n">
         <v>21</v>
@@ -20723,7 +20864,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="85" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D11" s="86" t="n">
         <v>42835</v>
@@ -20735,7 +20876,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="89" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="H11" s="90" t="n">
         <v>10.5</v>
@@ -20746,7 +20887,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D12" s="86" t="n">
         <v>42857</v>
@@ -20755,10 +20896,10 @@
         <v>42858</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="G12" s="89" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="H12" s="90" t="n">
         <v>14</v>
@@ -20769,7 +20910,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D13" s="86" t="n">
         <v>42835</v>
@@ -20781,7 +20922,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="89" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H13" s="90" t="n">
         <v>29.4</v>
@@ -20792,7 +20933,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="85" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="D14" s="86" t="n">
         <v>42839</v>
@@ -20804,7 +20945,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H14" s="90" t="n">
         <v>21</v>
@@ -20815,7 +20956,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="85" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D15" s="86" t="n">
         <v>42844</v>
@@ -20827,7 +20968,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H15" s="90" t="n">
         <v>28</v>
@@ -20838,7 +20979,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D16" s="86" t="n">
         <v>42844</v>
@@ -20850,7 +20991,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H16" s="90" t="n">
         <v>14</v>
@@ -20861,7 +21002,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="85" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D17" s="86" t="n">
         <v>42846</v>
@@ -20873,7 +21014,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H17" s="90" t="n">
         <v>7</v>
@@ -20884,7 +21025,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="85" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D18" s="86" t="n">
         <v>42850</v>
@@ -20893,10 +21034,10 @@
         <v>42851</v>
       </c>
       <c r="F18" s="91" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G18" s="89" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H18" s="90" t="n">
         <v>14</v>
@@ -20907,7 +21048,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="85" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D19" s="86" t="n">
         <v>42839</v>
@@ -20919,7 +21060,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H19" s="90" t="n">
         <v>21</v>
@@ -20930,7 +21071,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="85" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D20" s="86" t="n">
         <v>42850</v>
@@ -20942,7 +21083,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="89" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H20" s="90" t="n">
         <v>14</v>
@@ -20953,7 +21094,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="85" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D21" s="86" t="n">
         <v>42852</v>
@@ -20962,10 +21103,10 @@
         <v>42856</v>
       </c>
       <c r="F21" s="91" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="G21" s="89" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H21" s="90" t="n">
         <v>21</v>
@@ -20976,7 +21117,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D22" s="86" t="n">
         <v>42832</v>
@@ -20997,7 +21138,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D23" s="86" t="n">
         <v>42839</v>
@@ -21018,7 +21159,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D24" s="86" t="n">
         <v>42864</v>
@@ -21039,7 +21180,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="93" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="D25" s="94" t="n">
         <v>42864</v>
@@ -21107,7 +21248,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="40.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="55.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="13.29"/>
@@ -21188,31 +21329,31 @@
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="104" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C6" s="105" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="D6" s="105" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="E6" s="105" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="G6" s="105" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="H6" s="105" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="I6" s="106" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21288,7 +21429,7 @@
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="114"/>
       <c r="B12" s="115" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C12" s="109" t="n">
         <f aca="false">SUM(C7:C11)</f>
@@ -21318,31 +21459,31 @@
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="121" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="E15" s="105" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="F15" s="105" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="G15" s="105" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="H15" s="105" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="I15" s="106" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21418,7 +21559,7 @@
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="126"/>
       <c r="B21" s="115" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C21" s="109" t="n">
         <f aca="false">SUM(C16:C20)</f>
@@ -21543,7 +21684,7 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="135" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B5" s="136"/>
       <c r="C5" s="137"/>
@@ -21552,10 +21693,10 @@
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="138" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B6" s="139" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C6" s="137"/>
       <c r="D6" s="137"/>
@@ -21598,7 +21739,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A12" s="135" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B12" s="136"/>
       <c r="C12" s="137"/>
@@ -21607,10 +21748,10 @@
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="138" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B13" s="139" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C13" s="137"/>
       <c r="D13" s="137"/>
@@ -21653,7 +21794,7 @@
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A19" s="145" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B19" s="137"/>
       <c r="C19" s="137"/>
@@ -21991,34 +22132,34 @@
     </row>
     <row r="5" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="147" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B5" s="147" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C5" s="147" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D5" s="147" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E5" s="147" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="F5" s="147" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="G5" s="147" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="H5" s="147" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="I5" s="147" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="J5" s="148" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="K5" s="149"/>
       <c r="L5" s="149"/>

</xml_diff>

<commit_message>
Version finale rendu 9 février fichier de bord "Dorian"
</commit_message>
<xml_diff>
--- a/gestion_de_projet/Pilotage_de_projet.xlsx
+++ b/gestion_de_projet/Pilotage_de_projet.xlsx
@@ -173,10 +173,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="219">
   <si>
-    <t xml:space="preserve">TamairOS V0.1</t>
+    <t xml:space="preserve">Cosinus V0.1</t>
   </si>
   <si>
-    <t xml:space="preserve">TamairOS</t>
+    <t xml:space="preserve">Cosinus</t>
   </si>
   <si>
     <t xml:space="preserve">Projet</t>
@@ -342,8 +342,7 @@
     <t xml:space="preserve">GP003</t>
   </si>
   <si>
-    <t xml:space="preserve">L’équipe doit livrer le canevas instancié complété avec l’avancement à la date courante (Onglets 23a,23b,23c,23d,23e,23f,3a)
-Avant TD5</t>
+    <t xml:space="preserve">it</t>
   </si>
   <si>
     <t xml:space="preserve">GP004</t>
@@ -1394,7 +1393,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
@@ -1432,7 +1430,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
@@ -8861,9 +8858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>666720</xdr:colOff>
+      <xdr:colOff>666360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8872,8 +8869,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="353520" y="95040"/>
-          <a:ext cx="7901280" cy="331920"/>
+          <a:off x="352800" y="95040"/>
+          <a:ext cx="7897680" cy="331560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8925,9 +8922,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>819720</xdr:rowOff>
+      <xdr:rowOff>819360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8936,8 +8933,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13149360" y="3502440"/>
-          <a:ext cx="2895840" cy="557640"/>
+          <a:off x="13143600" y="3502440"/>
+          <a:ext cx="2895480" cy="557280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -8998,9 +8995,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>186480</xdr:colOff>
+      <xdr:colOff>186120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>519840</xdr:rowOff>
+      <xdr:rowOff>519480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9009,8 +9006,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13087440" y="4464360"/>
-          <a:ext cx="2895840" cy="552960"/>
+          <a:off x="13081680" y="4464360"/>
+          <a:ext cx="2895480" cy="552600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9071,9 +9068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>281520</xdr:colOff>
+      <xdr:colOff>281160</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>709920</xdr:rowOff>
+      <xdr:rowOff>709560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9082,8 +9079,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13182480" y="2476080"/>
-          <a:ext cx="2895840" cy="557640"/>
+          <a:off x="13176720" y="2476080"/>
+          <a:ext cx="2895480" cy="557280"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9144,9 +9141,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>207720</xdr:colOff>
+      <xdr:colOff>207360</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9155,8 +9152,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13108680" y="1736640"/>
-          <a:ext cx="2895840" cy="560520"/>
+          <a:off x="13102920" y="1736640"/>
+          <a:ext cx="2895480" cy="560160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9217,9 +9214,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>264600</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9228,8 +9225,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13165920" y="1355400"/>
-          <a:ext cx="2895840" cy="264960"/>
+          <a:off x="13160160" y="1355400"/>
+          <a:ext cx="2895480" cy="264600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9290,9 +9287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>33840</xdr:colOff>
+      <xdr:colOff>33480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9301,8 +9298,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16406280" y="559080"/>
-          <a:ext cx="3462840" cy="447120"/>
+          <a:off x="16400520" y="559080"/>
+          <a:ext cx="3462480" cy="446760"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9363,9 +9360,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>105120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9374,8 +9371,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16404120" y="1103400"/>
-          <a:ext cx="3536640" cy="467280"/>
+          <a:off x="16398360" y="1103400"/>
+          <a:ext cx="3536280" cy="466920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9452,9 +9449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>688680</xdr:colOff>
+      <xdr:colOff>688320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9463,8 +9460,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16427880" y="47520"/>
-          <a:ext cx="3288240" cy="392760"/>
+          <a:off x="16422120" y="47520"/>
+          <a:ext cx="3288240" cy="392400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9530,9 +9527,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>236160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9541,8 +9538,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17943480" y="2253960"/>
-          <a:ext cx="3312720" cy="2735280"/>
+          <a:off x="17942760" y="2253960"/>
+          <a:ext cx="3312360" cy="2734920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9685,9 +9682,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>188640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9696,8 +9693,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15913440" y="326160"/>
-          <a:ext cx="3312720" cy="1166400"/>
+          <a:off x="15914160" y="326160"/>
+          <a:ext cx="3312360" cy="1166040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9783,9 +9780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>653040</xdr:colOff>
+      <xdr:colOff>652680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9794,8 +9791,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4008600" y="6831000"/>
-          <a:ext cx="3331440" cy="823680"/>
+          <a:off x="4007880" y="6831000"/>
+          <a:ext cx="3331080" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9856,9 +9853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>234000</xdr:colOff>
+      <xdr:colOff>233640</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>55440</xdr:rowOff>
+      <xdr:rowOff>55080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9867,8 +9864,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9192960" y="6900120"/>
-          <a:ext cx="3358080" cy="824760"/>
+          <a:off x="9192600" y="6900120"/>
+          <a:ext cx="3357360" cy="824400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9939,9 +9936,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>255600</xdr:colOff>
+      <xdr:colOff>255240</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9950,8 +9947,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13698000" y="6670800"/>
-          <a:ext cx="3312360" cy="823320"/>
+          <a:off x="13697280" y="6670800"/>
+          <a:ext cx="3312360" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10032,9 +10029,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10043,8 +10040,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14491080" y="2001600"/>
-          <a:ext cx="3312720" cy="843480"/>
+          <a:off x="14490720" y="2001600"/>
+          <a:ext cx="3312000" cy="843120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10120,9 +10117,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1057680</xdr:rowOff>
+      <xdr:rowOff>1057320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10131,8 +10128,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17149680" y="2899080"/>
-          <a:ext cx="3358080" cy="819720"/>
+          <a:off x="17150040" y="2899080"/>
+          <a:ext cx="3358080" cy="819360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10208,9 +10205,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1378080</xdr:colOff>
+      <xdr:colOff>1377720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10220,7 +10217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="525240" y="0"/>
-          <a:ext cx="10941480" cy="513000"/>
+          <a:ext cx="10941120" cy="512640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10272,9 +10269,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>319680</xdr:rowOff>
+      <xdr:rowOff>319320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10283,8 +10280,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17093880" y="969120"/>
-          <a:ext cx="2895840" cy="1744920"/>
+          <a:off x="17094600" y="969120"/>
+          <a:ext cx="2895120" cy="1744560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10350,9 +10347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>706680</xdr:colOff>
+      <xdr:colOff>706320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10361,8 +10358,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="348480" y="71280"/>
-          <a:ext cx="6937200" cy="373320"/>
+          <a:off x="347760" y="71280"/>
+          <a:ext cx="6936840" cy="372960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10414,9 +10411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>92880</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10425,8 +10422,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3454920" y="1841400"/>
-          <a:ext cx="1602000" cy="574200"/>
+          <a:off x="3454560" y="1841400"/>
+          <a:ext cx="1601280" cy="573840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10509,9 +10506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>673920</xdr:colOff>
+      <xdr:colOff>673560</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10520,8 +10517,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1532880" y="3922200"/>
-          <a:ext cx="1681560" cy="510120"/>
+          <a:off x="1532520" y="3922200"/>
+          <a:ext cx="1680840" cy="509760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10604,9 +10601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>275040</xdr:colOff>
+      <xdr:colOff>274680</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10615,8 +10612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4293000" y="3922200"/>
-          <a:ext cx="1753200" cy="510120"/>
+          <a:off x="4292280" y="3922200"/>
+          <a:ext cx="1753200" cy="509760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10699,9 +10696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10710,8 +10707,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6590520" y="3922200"/>
-          <a:ext cx="1745640" cy="510120"/>
+          <a:off x="6589800" y="3922200"/>
+          <a:ext cx="1745640" cy="509760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10788,7 +10785,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>647640</xdr:colOff>
+      <xdr:colOff>648000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -10796,7 +10793,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>101160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10805,8 +10802,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2568240" y="2232360"/>
-          <a:ext cx="1499040" cy="1876680"/>
+          <a:off x="2568600" y="2231640"/>
+          <a:ext cx="1498680" cy="1876320"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10839,15 +10836,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>103680</xdr:colOff>
+      <xdr:colOff>104400</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>211680</xdr:colOff>
+      <xdr:colOff>212040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10856,8 +10853,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="3967920" y="2712960"/>
-          <a:ext cx="1499040" cy="915840"/>
+          <a:off x="3967560" y="2712240"/>
+          <a:ext cx="1498680" cy="915480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10890,15 +10887,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>103680</xdr:colOff>
+      <xdr:colOff>104400</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>78120</xdr:colOff>
+      <xdr:colOff>78480</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10907,8 +10904,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5112720" y="1568160"/>
-          <a:ext cx="1499040" cy="3205440"/>
+          <a:off x="5112360" y="1567440"/>
+          <a:ext cx="1498680" cy="3205080"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10947,9 +10944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>564840</xdr:colOff>
+      <xdr:colOff>564480</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10958,8 +10955,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="551880" y="1850040"/>
-          <a:ext cx="1745640" cy="574200"/>
+          <a:off x="551160" y="1850040"/>
+          <a:ext cx="1745280" cy="573840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11053,8 +11050,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2298960" y="2129400"/>
-          <a:ext cx="1155960" cy="4320"/>
+          <a:off x="2298240" y="2129400"/>
+          <a:ext cx="1156320" cy="4320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -11089,7 +11086,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>664920</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>56880</xdr:rowOff>
     </xdr:to>
@@ -11100,8 +11097,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3974400" y="1049400"/>
-          <a:ext cx="1654200" cy="571320"/>
+          <a:off x="3974040" y="1049400"/>
+          <a:ext cx="1653480" cy="571320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11163,9 +11160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>474480</xdr:colOff>
+      <xdr:colOff>474120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11174,8 +11171,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10665000" y="568440"/>
-          <a:ext cx="2850120" cy="1774440"/>
+          <a:off x="10664640" y="568440"/>
+          <a:ext cx="2849760" cy="1774080"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -11241,9 +11238,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>737280</xdr:colOff>
+      <xdr:colOff>736920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11252,8 +11249,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="203760" y="48240"/>
-          <a:ext cx="7112520" cy="373320"/>
+          <a:off x="203040" y="48240"/>
+          <a:ext cx="7112160" cy="372960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11305,9 +11302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>530280</xdr:colOff>
+      <xdr:colOff>529920</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11316,8 +11313,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3891960" y="1475640"/>
-          <a:ext cx="1602000" cy="358200"/>
+          <a:off x="3891600" y="1475640"/>
+          <a:ext cx="1601280" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11381,9 +11378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>639720</xdr:colOff>
+      <xdr:colOff>639360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11392,8 +11389,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2776680" y="2296440"/>
-          <a:ext cx="1211040" cy="365400"/>
+          <a:off x="2775960" y="2296440"/>
+          <a:ext cx="1211040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11457,9 +11454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>440280</xdr:colOff>
+      <xdr:colOff>439920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11468,8 +11465,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5000400" y="2296440"/>
-          <a:ext cx="1211040" cy="365760"/>
+          <a:off x="4999680" y="2296440"/>
+          <a:ext cx="1211040" cy="365400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11533,9 +11530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>199080</xdr:colOff>
+      <xdr:colOff>198720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11544,8 +11541,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6332760" y="2293200"/>
-          <a:ext cx="1253160" cy="350280"/>
+          <a:off x="6332400" y="2293200"/>
+          <a:ext cx="1252440" cy="349920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11603,7 +11600,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>44280</xdr:colOff>
+      <xdr:colOff>44640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11611,7 +11608,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>537840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11620,8 +11617,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3812400" y="1414440"/>
-          <a:ext cx="459360" cy="1301400"/>
+          <a:off x="3812400" y="1413720"/>
+          <a:ext cx="459000" cy="1300680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11654,7 +11651,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11662,7 +11659,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>628920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11671,8 +11668,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="4914360" y="1617120"/>
-          <a:ext cx="459360" cy="896040"/>
+          <a:off x="4914360" y="1616400"/>
+          <a:ext cx="459000" cy="895680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11705,15 +11702,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>540360</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>378360</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11722,8 +11719,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5598720" y="933120"/>
-          <a:ext cx="455760" cy="2260800"/>
+          <a:off x="5598360" y="932400"/>
+          <a:ext cx="455400" cy="2260440"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11762,7 +11759,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>530280</xdr:colOff>
+      <xdr:colOff>529920</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
@@ -11773,8 +11770,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3880800" y="927720"/>
-          <a:ext cx="1613160" cy="318240"/>
+          <a:off x="3880440" y="927720"/>
+          <a:ext cx="1612440" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11826,9 +11823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11837,8 +11834,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="2807640"/>
-          <a:ext cx="1211400" cy="350280"/>
+          <a:off x="3614040" y="2807640"/>
+          <a:ext cx="1210680" cy="349920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11902,9 +11899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11913,8 +11910,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="3807720"/>
-          <a:ext cx="1211400" cy="366120"/>
+          <a:off x="3614040" y="3807720"/>
+          <a:ext cx="1210680" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11978,9 +11975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11989,8 +11986,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="3311280"/>
-          <a:ext cx="1211400" cy="358560"/>
+          <a:off x="3614040" y="3311280"/>
+          <a:ext cx="1210680" cy="358200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12048,15 +12045,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12065,8 +12062,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="2666160"/>
-          <a:ext cx="221760" cy="321840"/>
+          <a:off x="3393000" y="2666520"/>
+          <a:ext cx="221400" cy="321480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12097,15 +12094,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12114,8 +12111,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="2666160"/>
-          <a:ext cx="221760" cy="1329840"/>
+          <a:off x="3393000" y="2666520"/>
+          <a:ext cx="221400" cy="1329480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12146,13 +12143,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
@@ -12163,8 +12160,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="2666160"/>
-          <a:ext cx="221760" cy="826200"/>
+          <a:off x="3393000" y="2666880"/>
+          <a:ext cx="221400" cy="825840"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12201,9 +12198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>581760</xdr:colOff>
+      <xdr:colOff>581400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12212,8 +12209,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10772280" y="375480"/>
-          <a:ext cx="2850120" cy="974520"/>
+          <a:off x="10771920" y="375480"/>
+          <a:ext cx="2849760" cy="974160"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -12274,9 +12271,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>472680</xdr:colOff>
+      <xdr:colOff>472320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12285,8 +12282,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="993960" y="2309040"/>
-          <a:ext cx="1211400" cy="365400"/>
+          <a:off x="993600" y="2309040"/>
+          <a:ext cx="1210680" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12350,9 +12347,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12361,8 +12358,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1827360" y="2809800"/>
-          <a:ext cx="1211400" cy="350280"/>
+          <a:off x="1826640" y="2809800"/>
+          <a:ext cx="1211040" cy="349920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12420,13 +12417,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>656280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
@@ -12437,8 +12434,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2678760"/>
-          <a:ext cx="248040" cy="307800"/>
+          <a:off x="1580400" y="2679480"/>
+          <a:ext cx="247320" cy="307440"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12475,9 +12472,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>531720</xdr:colOff>
+      <xdr:colOff>531360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12486,8 +12483,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1860840" y="3309840"/>
-          <a:ext cx="1211400" cy="350640"/>
+          <a:off x="1860120" y="3309840"/>
+          <a:ext cx="1211040" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12551,9 +12548,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>541440</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12562,8 +12559,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1870560" y="3893040"/>
-          <a:ext cx="1211400" cy="350640"/>
+          <a:off x="1869840" y="3893040"/>
+          <a:ext cx="1211040" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12627,9 +12624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>598320</xdr:colOff>
+      <xdr:colOff>597960</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12638,8 +12635,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1927440" y="4493160"/>
-          <a:ext cx="1211400" cy="350640"/>
+          <a:off x="1926720" y="4493160"/>
+          <a:ext cx="1211040" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12703,9 +12700,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:colOff>76680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12714,8 +12711,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7822440" y="2294640"/>
-          <a:ext cx="1256760" cy="365400"/>
+          <a:off x="7821720" y="2294640"/>
+          <a:ext cx="1256400" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12779,9 +12776,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>114840</xdr:colOff>
+      <xdr:colOff>114480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12790,8 +12787,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8667720" y="2878920"/>
-          <a:ext cx="1257120" cy="350280"/>
+          <a:off x="8667360" y="2878920"/>
+          <a:ext cx="1256400" cy="349920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12855,9 +12852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>124560</xdr:colOff>
+      <xdr:colOff>124200</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12866,8 +12863,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8677440" y="3402360"/>
-          <a:ext cx="1257120" cy="350640"/>
+          <a:off x="8677080" y="3402360"/>
+          <a:ext cx="1256400" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12925,9 +12922,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>260280</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -12942,8 +12939,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8454240" y="2664360"/>
-          <a:ext cx="214200" cy="391320"/>
+          <a:off x="8454600" y="2665080"/>
+          <a:ext cx="213840" cy="390960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12974,15 +12971,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>484200</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12991,57 +12988,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8454600" y="2664720"/>
-          <a:ext cx="223560" cy="915120"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:tailEnd len="med" type="arrow" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>655200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128880</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Connecteur en angle 32"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2678760"/>
-          <a:ext cx="281520" cy="808200"/>
+          <a:off x="8454960" y="2665080"/>
+          <a:ext cx="223200" cy="914760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13074,23 +13022,23 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>655560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>138600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:colOff>128880</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Connecteur en angle 33"/>
+        <xdr:cNvPr id="50" name="Connecteur en angle 32"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580400" y="2678400"/>
-          <a:ext cx="290880" cy="1391400"/>
+          <a:off x="1580040" y="2679480"/>
+          <a:ext cx="280800" cy="807840"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13121,25 +13069,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>86760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>195840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:colOff>138600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Connecteur en angle 34"/>
+        <xdr:cNvPr id="51" name="Connecteur en angle 33"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="2678760"/>
-          <a:ext cx="348120" cy="1991160"/>
+          <a:off x="1580400" y="2679120"/>
+          <a:ext cx="290160" cy="1391040"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13170,7 +13118,56 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
+      <xdr:colOff>656280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>87120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>196200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>20520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Connecteur en angle 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1580400" y="2679480"/>
+          <a:ext cx="347400" cy="1990800"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>655200</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -13178,7 +13175,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>538200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13187,8 +13184,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2900160" y="514080"/>
-          <a:ext cx="471600" cy="3114360"/>
+          <a:off x="2900160" y="513360"/>
+          <a:ext cx="471240" cy="3113640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13221,7 +13218,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>540360</xdr:colOff>
+      <xdr:colOff>540720</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -13229,7 +13226,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>258120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13238,8 +13235,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="6345720" y="186120"/>
-          <a:ext cx="457200" cy="3756240"/>
+          <a:off x="6345360" y="185040"/>
+          <a:ext cx="456840" cy="3756240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13278,9 +13275,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>530280</xdr:colOff>
+      <xdr:colOff>529920</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13289,8 +13286,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3891960" y="6193440"/>
-          <a:ext cx="1602000" cy="432360"/>
+          <a:off x="3891600" y="6193440"/>
+          <a:ext cx="1601280" cy="432000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13364,9 +13361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>639720</xdr:colOff>
+      <xdr:colOff>639360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13375,8 +13372,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2776680" y="7185240"/>
-          <a:ext cx="1211040" cy="443160"/>
+          <a:off x="2775960" y="7185240"/>
+          <a:ext cx="1211040" cy="442800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13434,7 +13431,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>44280</xdr:colOff>
+      <xdr:colOff>44640</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
@@ -13442,7 +13439,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>537840</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13451,8 +13448,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3764520" y="6254280"/>
-          <a:ext cx="555480" cy="1301400"/>
+          <a:off x="3764160" y="6255000"/>
+          <a:ext cx="555120" cy="1300680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13491,9 +13488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>195120</xdr:rowOff>
+      <xdr:rowOff>194760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13502,8 +13499,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="7804080"/>
-          <a:ext cx="1211400" cy="424080"/>
+          <a:off x="3614040" y="7804080"/>
+          <a:ext cx="1210680" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13543,9 +13540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13554,8 +13551,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="9015480"/>
-          <a:ext cx="1211400" cy="443160"/>
+          <a:off x="3614040" y="9015480"/>
+          <a:ext cx="1210680" cy="442800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13595,9 +13592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669960</xdr:colOff>
+      <xdr:colOff>669600</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13606,8 +13603,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3614400" y="8414280"/>
-          <a:ext cx="1211400" cy="434160"/>
+          <a:off x="3614040" y="8414280"/>
+          <a:ext cx="1210680" cy="433800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13641,13 +13638,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>210600</xdr:rowOff>
     </xdr:to>
@@ -13658,8 +13655,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="7633440"/>
-          <a:ext cx="221760" cy="389160"/>
+          <a:off x="3393000" y="7634160"/>
+          <a:ext cx="221400" cy="388800"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13690,13 +13687,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
@@ -13707,8 +13704,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="7633440"/>
-          <a:ext cx="221760" cy="1610280"/>
+          <a:off x="3393000" y="7634160"/>
+          <a:ext cx="221400" cy="1609920"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13739,13 +13736,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
@@ -13756,8 +13753,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393000" y="7633440"/>
-          <a:ext cx="221760" cy="999720"/>
+          <a:off x="3393000" y="7634160"/>
+          <a:ext cx="221400" cy="999360"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13794,9 +13791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>472680</xdr:colOff>
+      <xdr:colOff>472320</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13805,8 +13802,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="993960" y="7200720"/>
-          <a:ext cx="1211400" cy="442800"/>
+          <a:off x="993600" y="7200720"/>
+          <a:ext cx="1210680" cy="442440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13870,9 +13867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497880</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>197640</xdr:rowOff>
+      <xdr:rowOff>197280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13881,8 +13878,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1827360" y="7806600"/>
-          <a:ext cx="1211400" cy="424080"/>
+          <a:off x="1826640" y="7806600"/>
+          <a:ext cx="1211040" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13916,15 +13913,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>656280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>208440</xdr:rowOff>
+      <xdr:rowOff>208800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13933,8 +13930,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="7648560"/>
-          <a:ext cx="248040" cy="372240"/>
+          <a:off x="1580400" y="7648920"/>
+          <a:ext cx="247320" cy="371880"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13971,9 +13968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>531720</xdr:colOff>
+      <xdr:colOff>531360</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13982,8 +13979,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1860840" y="8412480"/>
-          <a:ext cx="1211400" cy="424440"/>
+          <a:off x="1860120" y="8412480"/>
+          <a:ext cx="1211040" cy="424080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14023,9 +14020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>541440</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:rowOff>183600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14034,8 +14031,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1870560" y="9118440"/>
-          <a:ext cx="1211400" cy="424440"/>
+          <a:off x="1869840" y="9118440"/>
+          <a:ext cx="1211040" cy="424080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14075,9 +14072,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>598320</xdr:colOff>
+      <xdr:colOff>597960</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14086,8 +14083,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1927440" y="9845280"/>
-          <a:ext cx="1211400" cy="424800"/>
+          <a:off x="1926720" y="9845280"/>
+          <a:ext cx="1211040" cy="424440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14121,9 +14118,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655200</xdr:colOff>
+      <xdr:colOff>655560</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -14138,8 +14135,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="7648560"/>
-          <a:ext cx="281520" cy="978120"/>
+          <a:off x="1580040" y="7649280"/>
+          <a:ext cx="280800" cy="977760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14170,15 +14167,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>138600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>194760</xdr:rowOff>
+      <xdr:rowOff>195120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14187,8 +14184,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580400" y="7648200"/>
-          <a:ext cx="290880" cy="1684800"/>
+          <a:off x="1580400" y="7648560"/>
+          <a:ext cx="290160" cy="1684440"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14219,13 +14216,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>656280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>195840</xdr:colOff>
+      <xdr:colOff>196200</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
@@ -14236,8 +14233,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580040" y="7649280"/>
-          <a:ext cx="348120" cy="2410920"/>
+          <a:off x="1580400" y="7650000"/>
+          <a:ext cx="347400" cy="2410560"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14268,7 +14265,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
+      <xdr:colOff>655200</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
@@ -14276,7 +14273,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>538200</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14285,8 +14282,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2850840" y="5355360"/>
-          <a:ext cx="570600" cy="3114360"/>
+          <a:off x="2850480" y="5356080"/>
+          <a:ext cx="570240" cy="3113640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -14319,15 +14316,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>541440</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>245880</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14336,8 +14333,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5484240" y="5839920"/>
-          <a:ext cx="552960" cy="2128320"/>
+          <a:off x="5483880" y="5839200"/>
+          <a:ext cx="552600" cy="2127960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -14376,9 +14373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:colOff>76680</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14387,8 +14384,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6206760" y="7183080"/>
-          <a:ext cx="1257120" cy="443160"/>
+          <a:off x="6206400" y="7183080"/>
+          <a:ext cx="1256400" cy="442800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14452,9 +14449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114840</xdr:colOff>
+      <xdr:colOff>114480</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14463,8 +14460,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7052040" y="7890840"/>
-          <a:ext cx="1257120" cy="424080"/>
+          <a:off x="7051320" y="7890840"/>
+          <a:ext cx="1257120" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14504,9 +14501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>124560</xdr:colOff>
+      <xdr:colOff>124200</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14515,8 +14512,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7061760" y="8525160"/>
-          <a:ext cx="1257120" cy="424440"/>
+          <a:off x="7061040" y="8525160"/>
+          <a:ext cx="1257120" cy="424080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14550,15 +14547,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>259920</xdr:colOff>
+      <xdr:colOff>260280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>474120</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14567,8 +14564,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6838560" y="7630920"/>
-          <a:ext cx="214200" cy="473040"/>
+          <a:off x="6838560" y="7631280"/>
+          <a:ext cx="213840" cy="472680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14599,15 +14596,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>260280</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>483840</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14616,8 +14613,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6838920" y="7631640"/>
-          <a:ext cx="223560" cy="1108080"/>
+          <a:off x="6838920" y="7632000"/>
+          <a:ext cx="223200" cy="1107720"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14659,9 +14656,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>760320</xdr:colOff>
+      <xdr:colOff>759960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14670,8 +14667,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="241920" y="78840"/>
-          <a:ext cx="7097400" cy="373320"/>
+          <a:off x="241200" y="78840"/>
+          <a:ext cx="7097040" cy="372960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14723,9 +14720,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>673920</xdr:colOff>
+      <xdr:colOff>673560</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14734,8 +14731,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4028040" y="1428120"/>
-          <a:ext cx="1609560" cy="350640"/>
+          <a:off x="4027680" y="1428120"/>
+          <a:ext cx="1608840" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14799,9 +14796,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>601560</xdr:colOff>
+      <xdr:colOff>601200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14810,8 +14807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1930680" y="2256480"/>
-          <a:ext cx="1211400" cy="349920"/>
+          <a:off x="1929960" y="2256480"/>
+          <a:ext cx="1211040" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14875,9 +14872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>396360</xdr:colOff>
+      <xdr:colOff>396000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14886,8 +14883,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4125600" y="2256480"/>
-          <a:ext cx="1234440" cy="573480"/>
+          <a:off x="4125240" y="2256480"/>
+          <a:ext cx="1233720" cy="573120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14970,9 +14967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>509760</xdr:colOff>
+      <xdr:colOff>509400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14981,8 +14978,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5866560" y="2245680"/>
-          <a:ext cx="1222200" cy="357840"/>
+          <a:off x="5866200" y="2245680"/>
+          <a:ext cx="1221480" cy="357480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15040,7 +15037,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6840</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -15048,7 +15045,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15057,8 +15054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3454200" y="871920"/>
-          <a:ext cx="474480" cy="2290680"/>
+          <a:off x="3454560" y="871200"/>
+          <a:ext cx="474120" cy="2290320"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15091,7 +15088,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>585720</xdr:colOff>
+      <xdr:colOff>586080</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -15099,7 +15096,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>682200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15108,8 +15105,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="4552560" y="1969200"/>
-          <a:ext cx="474480" cy="96480"/>
+          <a:off x="4551480" y="1968480"/>
+          <a:ext cx="474120" cy="96120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15142,15 +15139,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>684360</xdr:colOff>
+      <xdr:colOff>685080</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>689760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15159,8 +15156,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5418000" y="1201680"/>
-          <a:ext cx="463680" cy="1620360"/>
+          <a:off x="5418360" y="1200960"/>
+          <a:ext cx="463320" cy="1620360"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15199,7 +15196,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>752760</xdr:colOff>
+      <xdr:colOff>752400</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
@@ -15210,8 +15207,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4024440" y="887400"/>
-          <a:ext cx="1692000" cy="318240"/>
+          <a:off x="4024080" y="887400"/>
+          <a:ext cx="1691280" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15263,9 +15260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>623880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15274,8 +15271,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2768760" y="2759760"/>
-          <a:ext cx="1203480" cy="358200"/>
+          <a:off x="2768040" y="2759760"/>
+          <a:ext cx="1203480" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15339,9 +15336,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>623880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15350,8 +15347,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2768760" y="3767760"/>
-          <a:ext cx="1203480" cy="358200"/>
+          <a:off x="2768040" y="3767760"/>
+          <a:ext cx="1203480" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15415,9 +15412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>623880</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15426,8 +15423,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2768760" y="3263760"/>
-          <a:ext cx="1203480" cy="358200"/>
+          <a:off x="2768040" y="3263760"/>
+          <a:ext cx="1203480" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15485,15 +15482,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15502,8 +15499,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547360" y="2610720"/>
-          <a:ext cx="221760" cy="329760"/>
+          <a:off x="2547000" y="2611080"/>
+          <a:ext cx="221400" cy="329400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15534,15 +15531,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15551,8 +15548,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547360" y="2610720"/>
-          <a:ext cx="221760" cy="1337760"/>
+          <a:off x="2547000" y="2611080"/>
+          <a:ext cx="221400" cy="1337400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15583,13 +15580,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
@@ -15600,8 +15597,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547360" y="2611080"/>
-          <a:ext cx="221760" cy="833400"/>
+          <a:off x="2547000" y="2611800"/>
+          <a:ext cx="221400" cy="833040"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15638,9 +15635,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>418680</xdr:colOff>
+      <xdr:colOff>418320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15649,8 +15646,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4986360" y="2975760"/>
-          <a:ext cx="1203480" cy="350640"/>
+          <a:off x="4985640" y="2975760"/>
+          <a:ext cx="1203480" cy="350280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15714,9 +15711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>418680</xdr:colOff>
+      <xdr:colOff>418320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15725,8 +15722,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4986360" y="3480120"/>
-          <a:ext cx="1203480" cy="358200"/>
+          <a:off x="4985640" y="3480120"/>
+          <a:ext cx="1203480" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,9 +15787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
+      <xdr:colOff>478440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15801,8 +15798,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6643440" y="3930840"/>
-          <a:ext cx="1222200" cy="358560"/>
+          <a:off x="6642720" y="3930840"/>
+          <a:ext cx="1221840" cy="358200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15885,9 +15882,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
+      <xdr:colOff>478440</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15896,8 +15893,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6643440" y="2903760"/>
-          <a:ext cx="1222200" cy="358200"/>
+          <a:off x="6642720" y="2903760"/>
+          <a:ext cx="1221840" cy="357840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15961,9 +15958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
+      <xdr:colOff>478440</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -15972,8 +15969,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6643440" y="3367800"/>
-          <a:ext cx="1222200" cy="366120"/>
+          <a:off x="6642720" y="3367800"/>
+          <a:ext cx="1221840" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16050,13 +16047,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>586440</xdr:colOff>
+      <xdr:colOff>587160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>23400</xdr:colOff>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
@@ -16067,8 +16064,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4742280" y="2834280"/>
-          <a:ext cx="244800" cy="826200"/>
+          <a:off x="4741920" y="2835000"/>
+          <a:ext cx="244440" cy="825840"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16099,15 +16096,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>65160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16116,8 +16113,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462000" y="2607840"/>
-          <a:ext cx="182160" cy="476640"/>
+          <a:off x="6462000" y="2608200"/>
+          <a:ext cx="181440" cy="476280"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16148,13 +16145,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>586440</xdr:colOff>
+      <xdr:colOff>587160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>23400</xdr:colOff>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
@@ -16165,8 +16162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4742280" y="2834280"/>
-          <a:ext cx="244800" cy="322200"/>
+          <a:off x="4741920" y="2835000"/>
+          <a:ext cx="244440" cy="321840"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16197,9 +16194,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -16214,8 +16211,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462000" y="2607840"/>
-          <a:ext cx="182160" cy="948600"/>
+          <a:off x="6462000" y="2608560"/>
+          <a:ext cx="181440" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16246,9 +16243,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -16263,8 +16260,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462000" y="2607840"/>
-          <a:ext cx="182160" cy="1503720"/>
+          <a:off x="6462000" y="2608560"/>
+          <a:ext cx="181440" cy="1503360"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16301,9 +16298,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>55080</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16312,8 +16309,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="561240" y="2261520"/>
-          <a:ext cx="1226520" cy="365400"/>
+          <a:off x="560520" y="2261520"/>
+          <a:ext cx="1226160" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16371,7 +16368,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -16379,7 +16376,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16388,8 +16385,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2767680" y="189360"/>
-          <a:ext cx="479520" cy="3660480"/>
+          <a:off x="2767320" y="189000"/>
+          <a:ext cx="479160" cy="3659760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -16428,9 +16425,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>569880</xdr:colOff>
+      <xdr:colOff>569520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>331560</xdr:rowOff>
+      <xdr:rowOff>331200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16439,8 +16436,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11105640" y="3337560"/>
-          <a:ext cx="3312720" cy="1815480"/>
+          <a:off x="11105280" y="3337560"/>
+          <a:ext cx="3312000" cy="1815120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16525,9 +16522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>661320</xdr:colOff>
+      <xdr:colOff>660960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16536,8 +16533,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="554400" y="56160"/>
-          <a:ext cx="8424720" cy="373320"/>
+          <a:off x="553680" y="56160"/>
+          <a:ext cx="8423640" cy="372960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16589,9 +16586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1127520</xdr:colOff>
+      <xdr:colOff>1127160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -16604,8 +16601,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="117360" y="5010120"/>
-          <a:ext cx="10527480" cy="4280400"/>
+          <a:off x="116640" y="5010120"/>
+          <a:ext cx="10526400" cy="4280040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16626,9 +16623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>295920</xdr:colOff>
+      <xdr:colOff>295560</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16637,8 +16634,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12927600" y="3821760"/>
-          <a:ext cx="3330720" cy="2107800"/>
+          <a:off x="12926160" y="3821760"/>
+          <a:ext cx="3330720" cy="2107440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16752,9 +16749,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3883320</xdr:colOff>
+      <xdr:colOff>3882960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16764,7 +16761,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1899720" y="130680"/>
-          <a:ext cx="8239320" cy="376920"/>
+          <a:ext cx="8238960" cy="376560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16816,9 +16813,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>81720</xdr:colOff>
+      <xdr:colOff>81360</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16827,8 +16824,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14338800" y="1082520"/>
-          <a:ext cx="3312720" cy="2001960"/>
+          <a:off x="14338080" y="1082520"/>
+          <a:ext cx="3312360" cy="2001600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16913,9 +16910,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>498240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -16925,7 +16922,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16142400" y="1338480"/>
-          <a:ext cx="3312720" cy="2074680"/>
+          <a:ext cx="3312360" cy="2074320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -17002,7 +16999,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17047,7 +17044,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17092,7 +17089,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17137,7 +17134,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17182,7 +17179,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17227,7 +17224,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17272,7 +17269,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17317,7 +17314,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17362,7 +17359,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17407,7 +17404,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17452,7 +17449,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17497,7 +17494,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232520" y="1218960"/>
+          <a:off x="13231440" y="1218960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -17531,9 +17528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -17542,8 +17539,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15538680" y="278640"/>
-          <a:ext cx="3358080" cy="2045160"/>
+          <a:off x="15537240" y="278640"/>
+          <a:ext cx="3357720" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -17608,8 +17605,8 @@
   </sheetPr>
   <dimension ref="B1:S25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O37" activeCellId="0" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17618,7 +17615,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="0.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="5" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="5" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.45"/>
   </cols>
@@ -17653,7 +17650,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="8" t="n">
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
@@ -17893,7 +17890,7 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
@@ -17901,11 +17898,11 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="6.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="6.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="7.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="31" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="31" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="31" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="31" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="30" width="26.56"/>
@@ -17915,7 +17912,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="173" t="str">
         <f aca="false">"LISTE DES DECISIONS au "&amp;TEXT(J2,"jj/mm/aaaa")</f>
-        <v>LISTE DES DECISIONS au 19/01/2022</v>
+        <v>LISTE DES DECISIONS au 31/01/2022</v>
       </c>
       <c r="B1" s="173"/>
       <c r="C1" s="173"/>
@@ -17927,7 +17924,7 @@
       <c r="I1" s="173"/>
       <c r="J1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="K1" s="34"/>
     </row>
@@ -17943,7 +17940,7 @@
       <c r="I2" s="173"/>
       <c r="J2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="K2" s="37"/>
     </row>
@@ -17959,7 +17956,7 @@
       <c r="I3" s="173"/>
       <c r="J3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="K3" s="40"/>
     </row>
@@ -18120,7 +18117,7 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -18143,7 +18140,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="147" t="str">
         <f aca="false">"DOCUMENTS PROJET au "&amp;TEXT(I2,"jj/mm/aaaa")</f>
-        <v>DOCUMENTS PROJET au 19/01/2022</v>
+        <v>DOCUMENTS PROJET au 31/01/2022</v>
       </c>
       <c r="B1" s="147"/>
       <c r="C1" s="147"/>
@@ -18154,7 +18151,7 @@
       <c r="H1" s="147"/>
       <c r="I1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="J1" s="34"/>
     </row>
@@ -18169,7 +18166,7 @@
       <c r="H2" s="147"/>
       <c r="I2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="J2" s="37"/>
     </row>
@@ -18184,7 +18181,7 @@
       <c r="H3" s="147"/>
       <c r="I3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="J3" s="40"/>
     </row>
@@ -18740,7 +18737,7 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
@@ -18748,7 +18745,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="32.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="76.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="19.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="26.56"/>
@@ -18758,13 +18755,13 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="194" t="str">
         <f aca="false">"LIVRABLES PROJET au "&amp;TEXT(D2,"jj/mm/aaaa")</f>
-        <v>LIVRABLES PROJET au 19/01/2022</v>
+        <v>LIVRABLES PROJET au 31/01/2022</v>
       </c>
       <c r="B1" s="194"/>
       <c r="C1" s="194"/>
       <c r="D1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="E1" s="34"/>
     </row>
@@ -18774,7 +18771,7 @@
       <c r="C2" s="194"/>
       <c r="D2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="E2" s="37"/>
     </row>
@@ -18784,7 +18781,7 @@
       <c r="C3" s="194"/>
       <c r="D3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="E3" s="40"/>
     </row>
@@ -18956,7 +18953,7 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T24" activeCellId="0" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -18964,7 +18961,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="1.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="30" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="16.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="30" width="11.45"/>
@@ -18978,7 +18975,7 @@
       <c r="A1" s="55"/>
       <c r="B1" s="196" t="str">
         <f aca="false">"PLANNING COURANT  au "&amp;TEXT(K2,"jj/mm/aaaa")</f>
-        <v>PLANNING COURANT  au 19/01/2022</v>
+        <v>PLANNING COURANT  au 31/01/2022</v>
       </c>
       <c r="C1" s="196"/>
       <c r="D1" s="196"/>
@@ -18990,7 +18987,7 @@
       <c r="J1" s="196"/>
       <c r="K1" s="58" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="L1" s="58"/>
       <c r="M1" s="58"/>
@@ -19007,7 +19004,7 @@
       <c r="J2" s="196"/>
       <c r="K2" s="61" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
@@ -19025,7 +19022,7 @@
       <c r="J3" s="196"/>
       <c r="K3" s="64" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
@@ -19793,18 +19790,18 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="19.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="85.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="28.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="85.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="31" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="31" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="26.56"/>
@@ -19814,7 +19811,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="194" t="str">
         <f aca="false">"BILAN au "&amp;TEXT(G2,"jj/mm/aaaa")</f>
-        <v>BILAN au 19/01/2022</v>
+        <v>BILAN au 31/01/2022</v>
       </c>
       <c r="B1" s="194"/>
       <c r="C1" s="194"/>
@@ -19823,7 +19820,7 @@
       <c r="F1" s="194"/>
       <c r="G1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="H1" s="34"/>
     </row>
@@ -19836,7 +19833,7 @@
       <c r="F2" s="194"/>
       <c r="G2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="H2" s="37"/>
     </row>
@@ -19849,7 +19846,7 @@
       <c r="F3" s="194"/>
       <c r="G3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="H3" s="40"/>
     </row>
@@ -19965,11 +19962,11 @@
   </sheetPr>
   <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
@@ -20009,18 +20006,18 @@
   </sheetPr>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="19.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="85.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="28.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="85.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="31" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="31" width="21.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="26.56"/>
@@ -20036,7 +20033,7 @@
       <c r="F1" s="33"/>
       <c r="G1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="H1" s="34"/>
     </row>
@@ -20049,7 +20046,7 @@
       <c r="F2" s="36"/>
       <c r="G2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="H2" s="37"/>
     </row>
@@ -20062,7 +20059,7 @@
       <c r="F3" s="39"/>
       <c r="G3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="H3" s="40"/>
     </row>
@@ -20125,7 +20122,7 @@
       </c>
       <c r="H9" s="49"/>
     </row>
-    <row r="10" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="10" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A10" s="50" t="s">
         <v>22</v>
       </c>
@@ -20152,7 +20149,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="11" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A11" s="50" t="s">
         <v>22</v>
       </c>
@@ -20172,7 +20169,7 @@
       <c r="G11" s="52"/>
       <c r="H11" s="53"/>
     </row>
-    <row r="12" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="12" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A12" s="50" t="s">
         <v>22</v>
       </c>
@@ -20192,7 +20189,7 @@
       <c r="G12" s="52"/>
       <c r="H12" s="53"/>
     </row>
-    <row r="13" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="13" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A13" s="50" t="s">
         <v>32</v>
       </c>
@@ -20219,7 +20216,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="14" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A14" s="50" t="s">
         <v>32</v>
       </c>
@@ -20246,7 +20243,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="15" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A15" s="50" t="s">
         <v>32</v>
       </c>
@@ -20266,7 +20263,7 @@
       <c r="G15" s="52"/>
       <c r="H15" s="53"/>
     </row>
-    <row r="16" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="16" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A16" s="50" t="s">
         <v>32</v>
       </c>
@@ -20286,7 +20283,7 @@
       <c r="G16" s="52"/>
       <c r="H16" s="53"/>
     </row>
-    <row r="17" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="17" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A17" s="50" t="s">
         <v>32</v>
       </c>
@@ -20306,7 +20303,7 @@
       <c r="G17" s="52"/>
       <c r="H17" s="53"/>
     </row>
-    <row r="18" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="18" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A18" s="50" t="s">
         <v>32</v>
       </c>
@@ -20326,7 +20323,7 @@
       <c r="G18" s="52"/>
       <c r="H18" s="53"/>
     </row>
-    <row r="19" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="19" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A19" s="50"/>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
@@ -20336,7 +20333,7 @@
       <c r="G19" s="52"/>
       <c r="H19" s="53"/>
     </row>
-    <row r="20" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="20" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A20" s="50" t="s">
         <v>46</v>
       </c>
@@ -20356,7 +20353,7 @@
       <c r="G20" s="52"/>
       <c r="H20" s="53"/>
     </row>
-    <row r="21" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="21" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A21" s="50" t="s">
         <v>46</v>
       </c>
@@ -20383,7 +20380,7 @@
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
     </row>
-    <row r="22" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="22" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A22" s="50" t="s">
         <v>46</v>
       </c>
@@ -20403,7 +20400,7 @@
       <c r="G22" s="52"/>
       <c r="H22" s="53"/>
     </row>
-    <row r="23" s="31" customFormat="true" ht="20.75" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+    <row r="23" s="31" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
       <c r="A23" s="50" t="s">
         <v>46</v>
       </c>
@@ -20449,7 +20446,7 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -20472,7 +20469,7 @@
       <c r="J1" s="57"/>
       <c r="K1" s="58" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="L1" s="58"/>
       <c r="M1" s="58"/>
@@ -20489,7 +20486,7 @@
       <c r="J2" s="60"/>
       <c r="K2" s="61" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
@@ -20506,7 +20503,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
@@ -20939,7 +20936,7 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -20962,7 +20959,7 @@
       <c r="J1" s="57"/>
       <c r="K1" s="58" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="L1" s="58"/>
       <c r="M1" s="58"/>
@@ -20979,7 +20976,7 @@
       <c r="J2" s="60"/>
       <c r="K2" s="61" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
@@ -20996,7 +20993,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
@@ -21588,7 +21585,7 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -21611,7 +21608,7 @@
       <c r="J1" s="57"/>
       <c r="K1" s="58" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="L1" s="58"/>
       <c r="M1" s="58"/>
@@ -21629,7 +21626,7 @@
       <c r="J2" s="60"/>
       <c r="K2" s="61" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
@@ -21647,7 +21644,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
@@ -22309,7 +22306,7 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -22317,7 +22314,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="1.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="30" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="16.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="30" width="11.45"/>
@@ -22340,7 +22337,7 @@
       <c r="J1" s="57"/>
       <c r="K1" s="58" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="L1" s="58"/>
       <c r="M1" s="58"/>
@@ -22357,7 +22354,7 @@
       <c r="J2" s="60"/>
       <c r="K2" s="61" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
@@ -22374,7 +22371,7 @@
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
@@ -22904,7 +22901,7 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -22916,7 +22913,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="30" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="30" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="30" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="30" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="30" width="19.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="30" width="11.45"/>
@@ -22925,7 +22922,7 @@
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="100" t="str">
         <f aca="false">"Risques / opportunités au "&amp;TEXT(F2,"jj/MM/AAAA")</f>
-        <v>Risques / opportunités au 19/01/2022</v>
+        <v>Risques / opportunités au 31/01/2022</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -22933,7 +22930,7 @@
       <c r="E1" s="100"/>
       <c r="F1" s="101" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="G1" s="101"/>
       <c r="H1" s="101"/>
@@ -22947,7 +22944,7 @@
       <c r="E2" s="100"/>
       <c r="F2" s="102" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="G2" s="102"/>
       <c r="H2" s="102"/>
@@ -22961,7 +22958,7 @@
       <c r="E3" s="100"/>
       <c r="F3" s="103" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
@@ -23271,7 +23268,7 @@
   </sheetPr>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -23288,7 +23285,7 @@
       <c r="A1" s="129"/>
       <c r="B1" s="130" t="str">
         <f aca="false">'1a-Identification Projet'!$L$1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="C1" s="131"/>
       <c r="D1" s="131"/>
@@ -23304,7 +23301,7 @@
       <c r="A2" s="132"/>
       <c r="B2" s="133" t="n">
         <f aca="false">'1a-Identification Projet'!$L$2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="C2" s="131"/>
       <c r="D2" s="131"/>
@@ -23320,7 +23317,7 @@
       <c r="A3" s="134"/>
       <c r="B3" s="135" t="str">
         <f aca="false">'1a-Identification Projet'!$L$3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="C3" s="131"/>
       <c r="D3" s="131"/>
@@ -23719,17 +23716,17 @@
   </sheetPr>
   <dimension ref="A1:BH14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="7.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="58.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="30" width="18.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="30" width="11.45"/>
@@ -23741,7 +23738,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="147" t="str">
         <f aca="false">"LISTE DES ACTIONS au "&amp;TEXT(I2,"jj/mm/aaaa")</f>
-        <v>LISTE DES ACTIONS au 19/01/2022</v>
+        <v>LISTE DES ACTIONS au 31/01/2022</v>
       </c>
       <c r="B1" s="147"/>
       <c r="C1" s="147"/>
@@ -23752,7 +23749,7 @@
       <c r="H1" s="147"/>
       <c r="I1" s="34" t="str">
         <f aca="false">'1a-Identification Projet'!$L1</f>
-        <v>TamairOS V0.1</v>
+        <v>Cosinus V0.1</v>
       </c>
       <c r="J1" s="34"/>
     </row>
@@ -23767,7 +23764,7 @@
       <c r="H2" s="147"/>
       <c r="I2" s="37" t="n">
         <f aca="false">'1a-Identification Projet'!$L2</f>
-        <v>44580</v>
+        <v>44592</v>
       </c>
       <c r="J2" s="37"/>
     </row>
@@ -23782,7 +23779,7 @@
       <c r="H3" s="147"/>
       <c r="I3" s="40" t="str">
         <f aca="false">'1a-Identification Projet'!$L3</f>
-        <v>TamairOS</v>
+        <v>Cosinus</v>
       </c>
       <c r="J3" s="40"/>
     </row>

</xml_diff>

<commit_message>
Avancement gestion de projet "Dorian"
</commit_message>
<xml_diff>
--- a/gestion_de_projet/Pilotage_de_projet.xlsx
+++ b/gestion_de_projet/Pilotage_de_projet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1a-Identification Projet" sheetId="1" state="visible" r:id="rId2"/>
@@ -911,7 +911,7 @@
     <numFmt numFmtId="200" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="201" formatCode="@"/>
   </numFmts>
-  <fonts count="83">
+  <fonts count="84">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1432,6 +1432,11 @@
       <sz val="18"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7022,47 +7027,47 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="76" fillId="38" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="77" fillId="38" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="76" fillId="38" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="77" fillId="38" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="76" fillId="38" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="77" fillId="38" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="76" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="77" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="77" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="78" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="196" fontId="76" fillId="38" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="196" fontId="77" fillId="38" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7082,7 +7087,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="77" fillId="39" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="78" fillId="39" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7118,7 +7123,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="77" fillId="39" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="78" fillId="39" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7146,15 +7151,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="78" fillId="34" borderId="45" xfId="969" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="79" fillId="34" borderId="45" xfId="969" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="79" fillId="34" borderId="29" xfId="969" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="80" fillId="34" borderId="45" xfId="969" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="80" fillId="34" borderId="29" xfId="969" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -7414,7 +7419,7 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="80" fillId="0" borderId="0" xfId="983" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="81" fillId="0" borderId="0" xfId="983" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7426,11 +7431,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="81" fillId="34" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="82" fillId="34" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="81" fillId="34" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="82" fillId="34" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7486,7 +7491,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="82" fillId="43" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="83" fillId="43" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7522,31 +7527,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="37" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="76" fillId="37" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="76" fillId="38" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="77" fillId="38" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="76" fillId="38" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="77" fillId="38" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="196" fontId="76" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="196" fontId="77" fillId="38" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="196" fontId="76" fillId="38" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="196" fontId="77" fillId="38" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8858,9 +8863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>666000</xdr:colOff>
+      <xdr:colOff>665640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8870,7 +8875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="352800" y="95040"/>
-          <a:ext cx="7893720" cy="331200"/>
+          <a:ext cx="7893360" cy="330840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8922,9 +8927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>247680</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>819000</xdr:rowOff>
+      <xdr:rowOff>818640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8934,7 +8939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13137840" y="3502440"/>
-          <a:ext cx="2895120" cy="556920"/>
+          <a:ext cx="2894760" cy="556560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -8995,9 +9000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>185760</xdr:colOff>
+      <xdr:colOff>185400</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>519120</xdr:rowOff>
+      <xdr:rowOff>518760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9007,7 +9012,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13075920" y="4464360"/>
-          <a:ext cx="2895120" cy="552240"/>
+          <a:ext cx="2894760" cy="551880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9068,9 +9073,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>280800</xdr:colOff>
+      <xdr:colOff>280440</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>709200</xdr:rowOff>
+      <xdr:rowOff>708840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9080,7 +9085,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13170960" y="2476080"/>
-          <a:ext cx="2895120" cy="556920"/>
+          <a:ext cx="2894760" cy="556560"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9141,9 +9146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
+      <xdr:colOff>206640</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9153,7 +9158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13097160" y="1736640"/>
-          <a:ext cx="2895120" cy="559800"/>
+          <a:ext cx="2894760" cy="559440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9214,9 +9219,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9226,7 +9231,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13154400" y="1355400"/>
-          <a:ext cx="2895120" cy="264240"/>
+          <a:ext cx="2894760" cy="263880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9287,9 +9292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
+      <xdr:colOff>32760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9299,7 +9304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16394760" y="559080"/>
-          <a:ext cx="3462120" cy="446400"/>
+          <a:ext cx="3461760" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9360,9 +9365,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>104760</xdr:colOff>
+      <xdr:colOff>104400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9372,7 +9377,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16392600" y="1103400"/>
-          <a:ext cx="3535920" cy="466560"/>
+          <a:ext cx="3535560" cy="466200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9449,9 +9454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>687960</xdr:colOff>
+      <xdr:colOff>687600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9461,7 +9466,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16416360" y="47520"/>
-          <a:ext cx="3287880" cy="392040"/>
+          <a:ext cx="3287520" cy="391680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9527,19 +9532,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>235800</xdr:colOff>
+      <xdr:colOff>235440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="127" name="Rectangle à coins arrondis 1"/>
+        <xdr:cNvPr id="137" name="Rectangle à coins arrondis 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17942760" y="2253960"/>
-          <a:ext cx="3312000" cy="2734560"/>
+          <a:ext cx="3311640" cy="2734200"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9682,19 +9687,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>188280</xdr:colOff>
+      <xdr:colOff>187920</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="128" name="Rectangle à coins arrondis 1"/>
+        <xdr:cNvPr id="138" name="Rectangle à coins arrondis 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15914880" y="326160"/>
-          <a:ext cx="3311640" cy="1165680"/>
+          <a:ext cx="3311280" cy="1165320"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9780,19 +9785,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>652320</xdr:colOff>
+      <xdr:colOff>651960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="Rectangle à coins arrondis 1"/>
+        <xdr:cNvPr id="139" name="Rectangle à coins arrondis 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007160" y="6831000"/>
-          <a:ext cx="3330720" cy="822960"/>
+          <a:ext cx="3330360" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9853,19 +9858,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
+      <xdr:colOff>232920</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>54720</xdr:rowOff>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="130" name="Rectangle à coins arrondis 2"/>
+        <xdr:cNvPr id="140" name="Rectangle à coins arrondis 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9191880" y="6900120"/>
-          <a:ext cx="3357000" cy="824040"/>
+          <a:ext cx="3356640" cy="823680"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9936,19 +9941,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>254880</xdr:colOff>
+      <xdr:colOff>254520</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="131" name="Rectangle à coins arrondis 3"/>
+        <xdr:cNvPr id="141" name="Rectangle à coins arrondis 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13696560" y="6670800"/>
-          <a:ext cx="3312000" cy="822600"/>
+          <a:ext cx="3311640" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10029,19 +10034,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>240120</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="132" name="Rectangle à coins arrondis 4"/>
+        <xdr:cNvPr id="142" name="Rectangle à coins arrondis 4"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14490000" y="2001600"/>
-          <a:ext cx="3312000" cy="842760"/>
+          <a:ext cx="3311640" cy="842400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10117,19 +10122,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>44640</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1056960</xdr:rowOff>
+      <xdr:rowOff>1056600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="133" name="Rectangle à coins arrondis 1"/>
+        <xdr:cNvPr id="143" name="Rectangle à coins arrondis 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17150760" y="2899080"/>
-          <a:ext cx="3357720" cy="819000"/>
+          <a:ext cx="3357360" cy="818640"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10205,9 +10210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1377360</xdr:colOff>
+      <xdr:colOff>1377000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>178560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10217,7 +10222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="525240" y="0"/>
-          <a:ext cx="10940760" cy="512280"/>
+          <a:ext cx="10940400" cy="511920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10269,9 +10274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>44640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>318960</xdr:rowOff>
+      <xdr:rowOff>318600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10281,7 +10286,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17095320" y="969120"/>
-          <a:ext cx="2894760" cy="1744200"/>
+          <a:ext cx="2894400" cy="1743840"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -10347,9 +10352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>705960</xdr:colOff>
+      <xdr:colOff>705600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10359,7 +10364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="347760" y="71280"/>
-          <a:ext cx="6936480" cy="372600"/>
+          <a:ext cx="6936120" cy="372240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10411,9 +10416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10423,7 +10428,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3454560" y="1841400"/>
-          <a:ext cx="1600920" cy="573480"/>
+          <a:ext cx="1600560" cy="573120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10506,9 +10511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>673200</xdr:colOff>
+      <xdr:colOff>672840</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10518,7 +10523,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1532520" y="3922200"/>
-          <a:ext cx="1680480" cy="509400"/>
+          <a:ext cx="1680120" cy="509040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10601,9 +10606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:colOff>273960</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10613,7 +10618,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4292280" y="3922200"/>
-          <a:ext cx="1752840" cy="509400"/>
+          <a:ext cx="1752480" cy="509040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10696,9 +10701,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>141120</xdr:colOff>
+      <xdr:colOff>140760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10708,7 +10713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6589800" y="3922200"/>
-          <a:ext cx="1745280" cy="509400"/>
+          <a:ext cx="1744920" cy="509040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10785,7 +10790,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>648360</xdr:colOff>
+      <xdr:colOff>648720</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -10793,7 +10798,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>101160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10802,8 +10807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2568240" y="2232360"/>
-          <a:ext cx="1498320" cy="1875960"/>
+          <a:off x="2569320" y="2231640"/>
+          <a:ext cx="1497960" cy="1875600"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10836,15 +10841,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104760</xdr:colOff>
+      <xdr:colOff>105480</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>212400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10853,8 +10858,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="3968280" y="2712960"/>
-          <a:ext cx="1498320" cy="915120"/>
+          <a:off x="3968640" y="2712240"/>
+          <a:ext cx="1497960" cy="914760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10887,15 +10892,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104760</xdr:colOff>
+      <xdr:colOff>105480</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>78480</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10904,8 +10909,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5113080" y="1568160"/>
-          <a:ext cx="1498320" cy="3204720"/>
+          <a:off x="5113440" y="1567440"/>
+          <a:ext cx="1497960" cy="3204360"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -10944,9 +10949,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>564120</xdr:colOff>
+      <xdr:colOff>563760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10956,7 +10961,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="551160" y="1850040"/>
-          <a:ext cx="1744920" cy="573480"/>
+          <a:ext cx="1744560" cy="573120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11086,7 +11091,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>664200</xdr:colOff>
+      <xdr:colOff>663840</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>56880</xdr:rowOff>
     </xdr:to>
@@ -11098,7 +11103,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3974040" y="1049400"/>
-          <a:ext cx="1653120" cy="571320"/>
+          <a:ext cx="1652760" cy="571320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11160,9 +11165,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>473760</xdr:colOff>
+      <xdr:colOff>473400</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11172,7 +11177,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10664640" y="568440"/>
-          <a:ext cx="2849400" cy="1773720"/>
+          <a:ext cx="2849040" cy="1773360"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -11238,9 +11243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>736560</xdr:colOff>
+      <xdr:colOff>736200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11250,7 +11255,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="203040" y="48240"/>
-          <a:ext cx="7111800" cy="372600"/>
+          <a:ext cx="7111440" cy="372240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11302,9 +11307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
+      <xdr:colOff>529200</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11314,7 +11319,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3891600" y="1475640"/>
-          <a:ext cx="1600920" cy="357480"/>
+          <a:ext cx="1600560" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11378,9 +11383,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>639000</xdr:colOff>
+      <xdr:colOff>638640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11390,7 +11395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2775960" y="2296440"/>
-          <a:ext cx="1210680" cy="364680"/>
+          <a:ext cx="1210320" cy="364320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11454,9 +11459,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>439560</xdr:colOff>
+      <xdr:colOff>439200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11466,7 +11471,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4999680" y="2296440"/>
-          <a:ext cx="1210680" cy="365040"/>
+          <a:ext cx="1210320" cy="364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11530,9 +11535,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>198360</xdr:colOff>
+      <xdr:colOff>198000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11542,7 +11547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6332400" y="2293200"/>
-          <a:ext cx="1252080" cy="349560"/>
+          <a:ext cx="1251720" cy="349200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11600,7 +11605,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11608,7 +11613,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>537840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11617,8 +11622,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3813480" y="1414440"/>
-          <a:ext cx="458640" cy="1300320"/>
+          <a:off x="3813120" y="1413720"/>
+          <a:ext cx="458280" cy="1299960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11651,7 +11656,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>542160</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -11659,7 +11664,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>629280</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11668,8 +11673,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="4914720" y="1617120"/>
-          <a:ext cx="458640" cy="895320"/>
+          <a:off x="4915440" y="1616400"/>
+          <a:ext cx="458280" cy="894960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11702,15 +11707,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>541440</xdr:colOff>
+      <xdr:colOff>542160</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>378720</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11719,8 +11724,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5599080" y="933120"/>
-          <a:ext cx="455040" cy="2260080"/>
+          <a:off x="5599440" y="932400"/>
+          <a:ext cx="454680" cy="2259720"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -11759,7 +11764,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
+      <xdr:colOff>529200</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
@@ -11771,7 +11776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3880440" y="927720"/>
-          <a:ext cx="1612080" cy="318240"/>
+          <a:ext cx="1611720" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11823,9 +11828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11835,7 +11840,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="2807640"/>
-          <a:ext cx="1210320" cy="349560"/>
+          <a:ext cx="1209960" cy="349200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11899,9 +11904,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11911,7 +11916,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="3807720"/>
-          <a:ext cx="1210320" cy="365400"/>
+          <a:ext cx="1209960" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11975,9 +11980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -11987,7 +11992,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="3311280"/>
-          <a:ext cx="1210320" cy="357840"/>
+          <a:ext cx="1209960" cy="357480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12045,15 +12050,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12062,8 +12067,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="2667240"/>
-          <a:ext cx="221040" cy="321120"/>
+          <a:off x="3394080" y="2667600"/>
+          <a:ext cx="220680" cy="320760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12094,15 +12099,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12111,8 +12116,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="2667240"/>
-          <a:ext cx="221040" cy="1329120"/>
+          <a:off x="3394080" y="2667600"/>
+          <a:ext cx="220680" cy="1328760"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12143,13 +12148,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
@@ -12160,8 +12165,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="2667240"/>
-          <a:ext cx="221040" cy="825480"/>
+          <a:off x="3394080" y="2667960"/>
+          <a:ext cx="220680" cy="825120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12198,9 +12203,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
+      <xdr:colOff>580680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12210,7 +12215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10771920" y="375480"/>
-          <a:ext cx="2849400" cy="973800"/>
+          <a:ext cx="2849040" cy="973440"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -12271,9 +12276,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12283,7 +12288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="993600" y="2309040"/>
-          <a:ext cx="1210320" cy="364680"/>
+          <a:ext cx="1209960" cy="364320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12347,9 +12352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
+      <xdr:colOff>497160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12359,7 +12364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1826640" y="2809800"/>
-          <a:ext cx="1210680" cy="349560"/>
+          <a:ext cx="1210320" cy="349200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12417,13 +12422,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>657360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
+      <xdr:colOff>96480</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
@@ -12434,8 +12439,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1581120" y="2679840"/>
-          <a:ext cx="246960" cy="307080"/>
+          <a:off x="1581480" y="2680560"/>
+          <a:ext cx="246600" cy="306720"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12472,9 +12477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>531000</xdr:colOff>
+      <xdr:colOff>530640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12484,7 +12489,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1860120" y="3309840"/>
-          <a:ext cx="1210680" cy="349920"/>
+          <a:ext cx="1210320" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12548,9 +12553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>540360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12560,7 +12565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1869840" y="3893040"/>
-          <a:ext cx="1210680" cy="349920"/>
+          <a:ext cx="1210320" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12624,9 +12629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>597600</xdr:colOff>
+      <xdr:colOff>597240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12636,7 +12641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1926720" y="4493160"/>
-          <a:ext cx="1210680" cy="349920"/>
+          <a:ext cx="1210320" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12700,9 +12705,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12712,7 +12717,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7821720" y="2294640"/>
-          <a:ext cx="1256040" cy="364680"/>
+          <a:ext cx="1255680" cy="364320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12776,9 +12781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>113760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12788,7 +12793,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8667360" y="2878920"/>
-          <a:ext cx="1256040" cy="349560"/>
+          <a:ext cx="1255680" cy="349200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12852,9 +12857,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>123840</xdr:colOff>
+      <xdr:colOff>123480</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12864,7 +12869,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8677080" y="3402360"/>
-          <a:ext cx="1256040" cy="349920"/>
+          <a:ext cx="1255680" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12922,9 +12927,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>261360</xdr:colOff>
+      <xdr:colOff>261720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -12939,8 +12944,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8454960" y="2665440"/>
-          <a:ext cx="213480" cy="390600"/>
+          <a:off x="8455680" y="2666160"/>
+          <a:ext cx="213120" cy="390240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -12971,15 +12976,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>261720</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>484560</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -12988,57 +12993,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8455320" y="2665800"/>
-          <a:ext cx="222840" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="4a7ebb"/>
-          </a:solidFill>
-          <a:tailEnd len="med" type="arrow" w="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>129240</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Connecteur en angle 32"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="1580400" y="2679840"/>
-          <a:ext cx="280440" cy="807480"/>
+          <a:off x="8456040" y="2666160"/>
+          <a:ext cx="222480" cy="914040"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13071,23 +13027,23 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>656640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>138960</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:colOff>129240</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Connecteur en angle 33"/>
+        <xdr:cNvPr id="50" name="Connecteur en angle 32"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580760" y="2679480"/>
-          <a:ext cx="289800" cy="1390680"/>
+          <a:off x="1581120" y="2680560"/>
+          <a:ext cx="280080" cy="807120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13118,25 +13074,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>657000</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:colOff>138960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Connecteur en angle 34"/>
+        <xdr:cNvPr id="51" name="Connecteur en angle 33"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1581120" y="2679840"/>
-          <a:ext cx="347040" cy="1990440"/>
+          <a:off x="1581480" y="2680200"/>
+          <a:ext cx="289440" cy="1390320"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13167,7 +13123,56 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>657360</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>196560</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>20880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Connecteur en angle 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1581480" y="2680560"/>
+          <a:ext cx="346680" cy="1990080"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -13175,7 +13180,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>538200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13184,8 +13189,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2901240" y="514080"/>
-          <a:ext cx="470880" cy="3113280"/>
+          <a:off x="2900880" y="513360"/>
+          <a:ext cx="470520" cy="3112920"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13218,7 +13223,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>541440</xdr:colOff>
+      <xdr:colOff>541800</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
@@ -13226,7 +13231,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>258480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13235,8 +13240,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="6345720" y="185760"/>
-          <a:ext cx="456480" cy="3755880"/>
+          <a:off x="6346440" y="185040"/>
+          <a:ext cx="456120" cy="3755520"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13275,9 +13280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
+      <xdr:colOff>529200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13287,7 +13292,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3891600" y="6193440"/>
-          <a:ext cx="1600920" cy="431640"/>
+          <a:ext cx="1600560" cy="431280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13361,9 +13366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>639000</xdr:colOff>
+      <xdr:colOff>638640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13373,7 +13378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2775960" y="7185240"/>
-          <a:ext cx="1210680" cy="442440"/>
+          <a:ext cx="1210320" cy="442080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13431,7 +13436,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
@@ -13439,7 +13444,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>537840</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13448,8 +13453,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3765240" y="6254280"/>
-          <a:ext cx="554760" cy="1300320"/>
+          <a:off x="3764880" y="6255000"/>
+          <a:ext cx="554400" cy="1299960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -13488,9 +13493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>194400</xdr:rowOff>
+      <xdr:rowOff>194040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13500,7 +13505,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="7804080"/>
-          <a:ext cx="1210320" cy="423360"/>
+          <a:ext cx="1209960" cy="423000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13528,6 +13533,22 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Couche 1</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -13540,9 +13561,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13552,7 +13573,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="9015480"/>
-          <a:ext cx="1210320" cy="442440"/>
+          <a:ext cx="1209960" cy="442080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13580,6 +13601,22 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Couche 3</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -13592,9 +13629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13604,7 +13641,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3614040" y="8414280"/>
-          <a:ext cx="1210320" cy="433440"/>
+          <a:ext cx="1209960" cy="433080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13632,19 +13669,35 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Couche 2</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>210960</xdr:rowOff>
     </xdr:to>
@@ -13655,8 +13708,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="7634520"/>
-          <a:ext cx="221040" cy="388440"/>
+          <a:off x="3394080" y="7635240"/>
+          <a:ext cx="220680" cy="388080"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13687,13 +13740,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
@@ -13704,8 +13757,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="7634520"/>
-          <a:ext cx="221040" cy="1609560"/>
+          <a:off x="3394080" y="7635240"/>
+          <a:ext cx="220680" cy="1609200"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13736,13 +13789,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>267120</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
@@ -13753,8 +13806,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3393720" y="7634520"/>
-          <a:ext cx="221040" cy="999000"/>
+          <a:off x="3394080" y="7635240"/>
+          <a:ext cx="220680" cy="998640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13791,9 +13844,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13803,7 +13856,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="993600" y="7200720"/>
-          <a:ext cx="1210320" cy="442080"/>
+          <a:ext cx="1209960" cy="441720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13867,9 +13920,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
+      <xdr:colOff>756000</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>196920</xdr:rowOff>
+      <xdr:rowOff>196560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13879,7 +13932,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1826640" y="7806600"/>
-          <a:ext cx="1210680" cy="423360"/>
+          <a:ext cx="1469160" cy="423000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13907,21 +13960,37 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>La capture du besoin</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>657360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
+      <xdr:colOff>96480</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
+      <xdr:rowOff>209160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13930,8 +13999,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1581120" y="7649640"/>
-          <a:ext cx="246960" cy="371520"/>
+          <a:off x="1581480" y="7650000"/>
+          <a:ext cx="246600" cy="371160"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -13968,9 +14037,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>531000</xdr:colOff>
+      <xdr:colOff>530640</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -13980,7 +14049,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1860120" y="8412480"/>
-          <a:ext cx="1210680" cy="423720"/>
+          <a:ext cx="1210320" cy="423360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14008,6 +14077,22 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Le référentiel projet</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -14020,9 +14105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>540360</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14032,7 +14117,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1869840" y="9118440"/>
-          <a:ext cx="1210680" cy="423720"/>
+          <a:ext cx="1210320" cy="423360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14060,21 +14145,37 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>L’avancement du projet</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>194760</xdr:colOff>
+      <xdr:colOff>155160</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>44280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>597600</xdr:colOff>
+      <xdr:colOff>557640</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14083,8 +14184,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1926720" y="9845280"/>
-          <a:ext cx="1210680" cy="424080"/>
+          <a:off x="1887120" y="9845280"/>
+          <a:ext cx="1210320" cy="423720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14112,15 +14213,31 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Le bilan du projet</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656280</xdr:colOff>
+      <xdr:colOff>656640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -14135,8 +14252,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580400" y="7649640"/>
-          <a:ext cx="280440" cy="977400"/>
+          <a:off x="1581120" y="7650360"/>
+          <a:ext cx="280080" cy="977040"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14167,15 +14284,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>657000</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>57960</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>138960</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>195120</xdr:rowOff>
+      <xdr:rowOff>195480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14184,8 +14301,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1580760" y="7649280"/>
-          <a:ext cx="289800" cy="1684080"/>
+          <a:off x="1581480" y="7649640"/>
+          <a:ext cx="289440" cy="1683720"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14216,13 +14333,13 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>657360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
+      <xdr:colOff>196560</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
@@ -14233,8 +14350,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1581120" y="7650360"/>
-          <a:ext cx="347040" cy="2410200"/>
+          <a:off x="1581480" y="7651080"/>
+          <a:ext cx="346680" cy="2409840"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14265,7 +14382,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>655560</xdr:colOff>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
@@ -14273,7 +14390,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>538200</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14282,8 +14399,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2851560" y="5355360"/>
-          <a:ext cx="569880" cy="3113280"/>
+          <a:off x="2851200" y="5356080"/>
+          <a:ext cx="569520" cy="3112920"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -14316,15 +14433,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>542520</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>246600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14333,8 +14450,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5484600" y="5839920"/>
-          <a:ext cx="552240" cy="2127600"/>
+          <a:off x="5484960" y="5839200"/>
+          <a:ext cx="551880" cy="2127240"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -14373,9 +14490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14385,7 +14502,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6206400" y="7183080"/>
-          <a:ext cx="1256040" cy="442440"/>
+          <a:ext cx="1255680" cy="442080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14449,9 +14566,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>479520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14461,7 +14578,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7051320" y="7890840"/>
-          <a:ext cx="1256760" cy="423360"/>
+          <a:ext cx="1622160" cy="423000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14489,6 +14606,22 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Produire une documentation Doxygen</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -14501,9 +14634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>123840</xdr:colOff>
+      <xdr:colOff>123480</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14513,7 +14646,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7061040" y="8525160"/>
-          <a:ext cx="1256760" cy="423720"/>
+          <a:ext cx="1256400" cy="423360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14541,21 +14674,37 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Espace de projet sous GitHub</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>261000</xdr:colOff>
+      <xdr:colOff>261360</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>474480</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14564,8 +14713,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6838920" y="7632000"/>
-          <a:ext cx="213480" cy="472320"/>
+          <a:off x="6839640" y="7632360"/>
+          <a:ext cx="213120" cy="471960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14596,15 +14745,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>261360</xdr:colOff>
+      <xdr:colOff>261720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>484200</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -14613,8 +14762,593 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6839280" y="7632720"/>
-          <a:ext cx="222840" cy="1107360"/>
+          <a:off x="6840000" y="7633080"/>
+          <a:ext cx="222480" cy="1107000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>273600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>57600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676080</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>57600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3621240" y="9637560"/>
+          <a:ext cx="1209960" cy="442080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3a5f8b"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Couche 4</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266760</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>6840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>669240</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3614400" y="10249920"/>
+          <a:ext cx="1209960" cy="442080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3a5f8b"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Couche 5</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>51120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268920</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>127440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="Connecteur en angle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3403440" y="7642440"/>
+          <a:ext cx="213120" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55440</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>51120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>91080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Connecteur en angle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3403080" y="7642440"/>
+          <a:ext cx="213120" cy="2859120"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>259560</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>162360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>662040</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>101520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3607200" y="10908360"/>
+          <a:ext cx="1209960" cy="442080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3a5f8b"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Programme d’analyse Java</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>246240</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>648720</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3593880" y="11553480"/>
+          <a:ext cx="1209960" cy="544680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3a5f8b"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Programme de fragmentation Java</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>239760</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>128880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33120</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Rectangle 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3587400" y="12215880"/>
+          <a:ext cx="1408680" cy="435960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3a5f8b"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>L’interface graphique en JAVA</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55080</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268200</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>29160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="Connecteur en angle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3402720" y="7642080"/>
+          <a:ext cx="213120" cy="3468240"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>52560</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>45000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>248400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>44280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Connecteur en angle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3400200" y="7635960"/>
+          <a:ext cx="195840" cy="4159800"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="4a7ebb"/>
+          </a:solidFill>
+          <a:tailEnd len="med" type="arrow" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>46080</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>64080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247680</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="89" name="Connecteur en angle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3393720" y="7655040"/>
+          <a:ext cx="201600" cy="4755960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -14656,19 +15390,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>759600</xdr:colOff>
+      <xdr:colOff>759240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="Text Box 2"/>
+        <xdr:cNvPr id="90" name="Text Box 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241200" y="78840"/>
-          <a:ext cx="7096680" cy="372600"/>
+          <a:ext cx="7096320" cy="372240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14720,19 +15454,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>673200</xdr:colOff>
+      <xdr:colOff>672840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="81" name="Rectangle 52"/>
+        <xdr:cNvPr id="91" name="Rectangle 52"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4027680" y="1428120"/>
-          <a:ext cx="1608480" cy="349920"/>
+          <a:ext cx="1608120" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14796,19 +15530,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>600840</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="82" name="Rectangle 53"/>
+        <xdr:cNvPr id="92" name="Rectangle 53"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1929960" y="2256480"/>
-          <a:ext cx="1210680" cy="349200"/>
+          <a:ext cx="1210320" cy="348840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14872,19 +15606,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>395280</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="83" name="Rectangle 54"/>
+        <xdr:cNvPr id="93" name="Rectangle 54"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4125240" y="2256480"/>
-          <a:ext cx="1233360" cy="572760"/>
+          <a:ext cx="1233000" cy="572400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14967,19 +15701,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>509040</xdr:colOff>
+      <xdr:colOff>508680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="84" name="Rectangle 55"/>
+        <xdr:cNvPr id="94" name="Rectangle 55"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5866200" y="2245680"/>
-          <a:ext cx="1221120" cy="357120"/>
+          <a:ext cx="1220760" cy="356760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15037,7 +15771,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7200</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -15045,17 +15779,17 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="85" name="Connecteur en angle 56"/>
+        <xdr:cNvPr id="95" name="Connecteur en angle 56"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="3454200" y="871920"/>
-          <a:ext cx="473760" cy="2289960"/>
+          <a:off x="3455280" y="871200"/>
+          <a:ext cx="473400" cy="2289600"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15088,7 +15822,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>586440</xdr:colOff>
+      <xdr:colOff>586800</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -15096,17 +15830,17 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>682200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="86" name="Connecteur en angle 57"/>
+        <xdr:cNvPr id="96" name="Connecteur en angle 57"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="4552560" y="1969200"/>
-          <a:ext cx="473760" cy="95760"/>
+          <a:off x="4552200" y="1968480"/>
+          <a:ext cx="473400" cy="95400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15139,25 +15873,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>685440</xdr:colOff>
+      <xdr:colOff>686160</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>689760</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="87" name="Connecteur en angle 58"/>
+        <xdr:cNvPr id="97" name="Connecteur en angle 58"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1" rot="16200000">
-          <a:off x="5419080" y="1201680"/>
-          <a:ext cx="462960" cy="1620000"/>
+          <a:off x="5419440" y="1200960"/>
+          <a:ext cx="462600" cy="1619640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -15196,19 +15930,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>752040</xdr:colOff>
+      <xdr:colOff>751680</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="88" name="ZoneTexte 39"/>
+        <xdr:cNvPr id="98" name="ZoneTexte 39"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4024080" y="887400"/>
-          <a:ext cx="1690920" cy="318240"/>
+          <a:ext cx="1690560" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15260,19 +15994,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
+      <xdr:colOff>623160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="89" name="Rectangle 60"/>
+        <xdr:cNvPr id="99" name="Rectangle 60"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2768040" y="2759760"/>
-          <a:ext cx="1203120" cy="357480"/>
+          <a:ext cx="1202760" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15336,19 +16070,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
+      <xdr:colOff>623160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="90" name="Rectangle 61"/>
+        <xdr:cNvPr id="100" name="Rectangle 61"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2768040" y="3767760"/>
-          <a:ext cx="1203120" cy="357480"/>
+          <a:ext cx="1202760" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15412,19 +16146,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>623520</xdr:colOff>
+      <xdr:colOff>623160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="91" name="Rectangle 62"/>
+        <xdr:cNvPr id="101" name="Rectangle 62"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2768040" y="3263760"/>
-          <a:ext cx="1203120" cy="357480"/>
+          <a:ext cx="1202760" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15482,25 +16216,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="Connecteur en angle 63"/>
+        <xdr:cNvPr id="102" name="Connecteur en angle 63"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547720" y="2611800"/>
-          <a:ext cx="221040" cy="329040"/>
+          <a:off x="2548080" y="2612160"/>
+          <a:ext cx="220680" cy="328680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15531,25 +16265,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="Connecteur en angle 64"/>
+        <xdr:cNvPr id="103" name="Connecteur en angle 64"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547720" y="2611800"/>
-          <a:ext cx="221040" cy="1337040"/>
+          <a:off x="2548080" y="2612160"/>
+          <a:ext cx="220680" cy="1336680"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15580,25 +16314,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="Connecteur en angle 65"/>
+        <xdr:cNvPr id="104" name="Connecteur en angle 65"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2547720" y="2612160"/>
-          <a:ext cx="221040" cy="832680"/>
+          <a:off x="2548080" y="2612880"/>
+          <a:ext cx="220680" cy="832320"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -15635,19 +16369,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>417960</xdr:colOff>
+      <xdr:colOff>417600</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="Rectangle 66"/>
+        <xdr:cNvPr id="105" name="Rectangle 66"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4985640" y="2975760"/>
-          <a:ext cx="1203120" cy="349920"/>
+          <a:ext cx="1202760" cy="349560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15711,19 +16445,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>417960</xdr:colOff>
+      <xdr:colOff>417600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="96" name="Rectangle 67"/>
+        <xdr:cNvPr id="106" name="Rectangle 67"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4985640" y="3480120"/>
-          <a:ext cx="1203120" cy="357480"/>
+          <a:ext cx="1202760" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15787,19 +16521,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478080</xdr:colOff>
+      <xdr:colOff>477720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="97" name="Rectangle 68"/>
+        <xdr:cNvPr id="107" name="Rectangle 68"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6642720" y="3930840"/>
-          <a:ext cx="1221480" cy="357840"/>
+          <a:ext cx="1221120" cy="357480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15882,19 +16616,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478080</xdr:colOff>
+      <xdr:colOff>477720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="98" name="Rectangle 69"/>
+        <xdr:cNvPr id="108" name="Rectangle 69"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6642720" y="2903760"/>
-          <a:ext cx="1221480" cy="357480"/>
+          <a:ext cx="1221120" cy="357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15958,19 +16692,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>478080</xdr:colOff>
+      <xdr:colOff>477720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="Rectangle 70"/>
+        <xdr:cNvPr id="109" name="Rectangle 70"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6642720" y="3367800"/>
-          <a:ext cx="1221480" cy="365400"/>
+          <a:ext cx="1221120" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16047,25 +16781,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>587520</xdr:colOff>
+      <xdr:colOff>588240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
+      <xdr:colOff>24120</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="100" name="Connecteur en angle 71"/>
+        <xdr:cNvPr id="110" name="Connecteur en angle 71"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4742640" y="2835360"/>
-          <a:ext cx="244080" cy="825480"/>
+          <a:off x="4743000" y="2836080"/>
+          <a:ext cx="243720" cy="825120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16096,25 +16830,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>691920</xdr:colOff>
+      <xdr:colOff>692280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>65520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="101" name="Connecteur en angle 72"/>
+        <xdr:cNvPr id="111" name="Connecteur en angle 72"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462360" y="2608920"/>
-          <a:ext cx="181080" cy="475920"/>
+          <a:off x="6463080" y="2609280"/>
+          <a:ext cx="180720" cy="475560"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16145,25 +16879,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>587520</xdr:colOff>
+      <xdr:colOff>588240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
+      <xdr:colOff>24120</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="Connecteur en angle 73"/>
+        <xdr:cNvPr id="112" name="Connecteur en angle 73"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="4742640" y="2835360"/>
-          <a:ext cx="244080" cy="321480"/>
+          <a:off x="4743000" y="2836080"/>
+          <a:ext cx="243720" cy="321120"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16194,9 +16928,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>691920</xdr:colOff>
+      <xdr:colOff>692280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -16206,13 +16940,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="103" name="Connecteur en angle 74"/>
+        <xdr:cNvPr id="113" name="Connecteur en angle 74"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462360" y="2608920"/>
-          <a:ext cx="181080" cy="947880"/>
+          <a:off x="6463080" y="2609640"/>
+          <a:ext cx="180720" cy="947520"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16243,9 +16977,9 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>691920</xdr:colOff>
+      <xdr:colOff>692280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -16255,13 +16989,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="Connecteur en angle 75"/>
+        <xdr:cNvPr id="114" name="Connecteur en angle 75"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6462360" y="2608920"/>
-          <a:ext cx="181080" cy="1503000"/>
+          <a:off x="6463080" y="2609640"/>
+          <a:ext cx="180720" cy="1502640"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -16298,19 +17032,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>54360</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="105" name="Rectangle 76"/>
+        <xdr:cNvPr id="115" name="Rectangle 76"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="560520" y="2261520"/>
-          <a:ext cx="1225800" cy="364680"/>
+          <a:ext cx="1225440" cy="364320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16368,7 +17102,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>253440</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
@@ -16376,17 +17110,17 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>681840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="Connecteur en angle 77"/>
+        <xdr:cNvPr id="116" name="Connecteur en angle 77"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1" rot="5400000">
-          <a:off x="2766960" y="189720"/>
-          <a:ext cx="478800" cy="3659400"/>
+          <a:off x="2768040" y="189000"/>
+          <a:ext cx="478440" cy="3659040"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -16425,19 +17159,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>569160</xdr:colOff>
+      <xdr:colOff>568800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>330840</xdr:rowOff>
+      <xdr:rowOff>330480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="Rectangle à coins arrondis 28"/>
+        <xdr:cNvPr id="117" name="Rectangle à coins arrondis 28"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11105280" y="3337560"/>
-          <a:ext cx="3311640" cy="1814760"/>
+          <a:ext cx="3311280" cy="1814400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16522,19 +17256,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>660600</xdr:colOff>
+      <xdr:colOff>660240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="108" name="Text Box 2"/>
+        <xdr:cNvPr id="118" name="Text Box 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="553680" y="56160"/>
-          <a:ext cx="8422560" cy="372600"/>
+          <a:ext cx="8422200" cy="372240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16586,13 +17320,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1126800</xdr:colOff>
+      <xdr:colOff>1126440</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="109" name="Image 28" descr=""/>
+        <xdr:cNvPr id="119" name="Image 28" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -16602,7 +17336,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="116640" y="5010120"/>
-          <a:ext cx="10525320" cy="4279680"/>
+          <a:ext cx="10524960" cy="4279320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16623,19 +17357,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>295200</xdr:colOff>
+      <xdr:colOff>294840</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="110" name="Rectangle à coins arrondis 3"/>
+        <xdr:cNvPr id="120" name="Rectangle à coins arrondis 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12925800" y="3821760"/>
-          <a:ext cx="3330000" cy="2107080"/>
+          <a:ext cx="3329640" cy="2106720"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16749,19 +17483,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3882600</xdr:colOff>
+      <xdr:colOff>3882240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="111" name="Text Box 2"/>
+        <xdr:cNvPr id="121" name="Text Box 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1899720" y="130680"/>
-          <a:ext cx="8238600" cy="376200"/>
+          <a:ext cx="8238240" cy="375840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16813,19 +17547,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>80640</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="112" name="Rectangle à coins arrondis 3"/>
+        <xdr:cNvPr id="122" name="Rectangle à coins arrondis 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14338080" y="1082520"/>
-          <a:ext cx="3312000" cy="2001240"/>
+          <a:ext cx="3311640" cy="2000880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16910,19 +17644,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>497880</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="113" name="Rectangle à coins arrondis 1"/>
+        <xdr:cNvPr id="123" name="Rectangle à coins arrondis 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16143120" y="1338480"/>
-          <a:ext cx="3312000" cy="2073960"/>
+          <a:ext cx="3311640" cy="2073600"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -16994,7 +17728,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="114" name="AutoShape 1" hidden="1"/>
+        <xdr:cNvPr id="124" name="AutoShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17039,7 +17773,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="115" name="AutoShape 2" hidden="1"/>
+        <xdr:cNvPr id="125" name="AutoShape 2" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17084,7 +17818,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="AutoShape 3" hidden="1"/>
+        <xdr:cNvPr id="126" name="AutoShape 3" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17129,7 +17863,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="117" name="AutoShape 4" hidden="1"/>
+        <xdr:cNvPr id="127" name="AutoShape 4" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17174,7 +17908,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="118" name="AutoShape 5" hidden="1"/>
+        <xdr:cNvPr id="128" name="AutoShape 5" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17219,7 +17953,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="AutoShape 6" hidden="1"/>
+        <xdr:cNvPr id="129" name="AutoShape 6" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17264,7 +17998,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="120" name="AutoShape 10" hidden="1"/>
+        <xdr:cNvPr id="130" name="AutoShape 10" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17309,7 +18043,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="121" name="AutoShape 11" hidden="1"/>
+        <xdr:cNvPr id="131" name="AutoShape 11" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17354,7 +18088,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="122" name="AutoShape 12" hidden="1"/>
+        <xdr:cNvPr id="132" name="AutoShape 12" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17399,7 +18133,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="123" name="AutoShape 13" hidden="1"/>
+        <xdr:cNvPr id="133" name="AutoShape 13" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17444,7 +18178,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="124" name="AutoShape 14" hidden="1"/>
+        <xdr:cNvPr id="134" name="AutoShape 14" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17489,7 +18223,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="125" name="AutoShape 15" hidden="1"/>
+        <xdr:cNvPr id="135" name="AutoShape 15" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17528,19 +18262,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
+      <xdr:colOff>9000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="126" name="Rectangle à coins arrondis 13"/>
+        <xdr:cNvPr id="136" name="Rectangle à coins arrondis 13"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15535800" y="278640"/>
-          <a:ext cx="3357720" cy="2044440"/>
+          <a:ext cx="3357360" cy="2044080"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -17606,7 +18340,7 @@
   <dimension ref="B1:S25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O37" activeCellId="0" sqref="O37"/>
+      <selection pane="topLeft" activeCell="O37" activeCellId="1" sqref="K29 O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17891,7 +18625,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
+      <selection pane="topLeft" activeCell="M26" activeCellId="1" sqref="K29 M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18118,7 +18852,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="K29 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
@@ -18738,7 +19472,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="1" sqref="K29 J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
@@ -18954,7 +19688,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T24" activeCellId="0" sqref="T24"/>
+      <selection pane="topLeft" activeCell="T24" activeCellId="1" sqref="K29 T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19791,7 +20525,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="1" sqref="K29 J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19963,10 +20697,10 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+      <selection pane="topLeft" activeCell="J32" activeCellId="1" sqref="K29 J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.89"/>
@@ -20006,8 +20740,8 @@
   </sheetPr>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="K29 E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
@@ -20447,7 +21181,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="1" sqref="K29 J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20937,7 +21671,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="1" sqref="K29 G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21585,8 +22319,8 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22307,7 +23041,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
+      <selection pane="topLeft" activeCell="D56" activeCellId="1" sqref="K29 D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22902,7 +23636,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="1" sqref="K29 B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23269,7 +24003,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="K29 H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -23717,7 +24451,7 @@
   <dimension ref="A1:BH14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
+      <selection pane="topLeft" activeCell="O29" activeCellId="1" sqref="K29 O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>